<commit_message>
Fechas de las ECU ajustadas al calendario respectivo
</commit_message>
<xml_diff>
--- a/documentos/General/CronogramaTSP.xlsx
+++ b/documentos/General/CronogramaTSP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Tarea</t>
   </si>
@@ -105,21 +105,6 @@
     <t>Especificacion casos de prueba</t>
   </si>
   <si>
-    <t>ECU. Registrar historial médico en forma local</t>
-  </si>
-  <si>
-    <t>ECU. Consultar historial médico de forma local</t>
-  </si>
-  <si>
-    <t>ECU. Modificar historial médico de forma local</t>
-  </si>
-  <si>
-    <t>ECU. Registrar historial médico desde internet</t>
-  </si>
-  <si>
-    <t>ECU. Modificar historial médico desde internet</t>
-  </si>
-  <si>
     <t>ECU. Modificar información básica MVZ's</t>
   </si>
   <si>
@@ -129,9 +114,6 @@
     <t>ECU. Modificar información básica pacientes</t>
   </si>
   <si>
-    <t>ECU. Consultar historial médico desde internet</t>
-  </si>
-  <si>
     <t>ECU. Reporte adminsitrativo</t>
   </si>
   <si>
@@ -166,13 +148,34 @@
   </si>
   <si>
     <t>ECU. Registrar MVZ's</t>
+  </si>
+  <si>
+    <t>ECU. Consultar historial médico</t>
+  </si>
+  <si>
+    <t>ECU. Modificar historial médico</t>
+  </si>
+  <si>
+    <t>Listas de chequeo - ECU Primera Semana</t>
+  </si>
+  <si>
+    <t>Listas de chequeo - ECU Segunda Semana</t>
+  </si>
+  <si>
+    <t>Listas de chequeo - ECU Tercera Semana</t>
+  </si>
+  <si>
+    <t>ECU. Registrar historial médico</t>
+  </si>
+  <si>
+    <t>Diccionario de Datos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,6 +207,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -225,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -259,8 +267,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="145">
+  <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -406,8 +453,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,15 +487,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="145">
+  <cellStyles count="155">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -511,6 +595,11 @@
     <cellStyle name="Hipervínculo" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -583,6 +672,11 @@
     <cellStyle name="Hipervínculo visitado" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -912,783 +1006,738 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I51"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" style="12" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="B3" s="6" t="s">
+      <c r="J2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="17">
+        <v>2</v>
+      </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="7">
+      <c r="G3" s="7"/>
+      <c r="H3" s="19">
         <v>1</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
-      <c r="B4" s="6" t="s">
+      <c r="J3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7">
+      <c r="D4" s="17">
         <v>4</v>
       </c>
-      <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="7">
+      <c r="G4" s="7"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="17">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="17">
         <v>1</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
-      <c r="B5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="9">
-        <v>4</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9">
-        <v>1</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
-      <c r="B6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9">
-        <v>1</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="9">
-        <v>2</v>
-      </c>
-      <c r="D7" s="9"/>
+      <c r="J6" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="18">
+        <v>2</v>
+      </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="9">
-        <v>1</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="D8" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="18">
+        <v>2</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="9">
-        <v>1</v>
-      </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="18">
+        <v>2</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="7">
-        <v>2</v>
-      </c>
-      <c r="D10" s="7"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="19">
+        <v>2</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="C10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="7">
-        <v>2</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="7">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7"/>
+      <c r="J10" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="C11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="7">
-        <v>2</v>
-      </c>
-      <c r="H11" s="7" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="7">
-        <v>2</v>
-      </c>
-      <c r="D12" s="7"/>
+      <c r="J11" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="C12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="7">
-        <v>2</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="7">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7"/>
+      <c r="J12" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="C13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="7">
-        <v>2</v>
-      </c>
-      <c r="H13" s="7" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9">
-      <c r="B14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="7">
-        <v>2</v>
-      </c>
-      <c r="D14" s="7"/>
+      <c r="J13" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="C14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="7">
-        <v>2</v>
-      </c>
-      <c r="H14" s="7" t="s">
+      <c r="G14" s="7"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="7">
-        <v>2</v>
-      </c>
-      <c r="D15" s="7"/>
+      <c r="J14" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="C15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="7">
-        <v>2</v>
-      </c>
-      <c r="H15" s="7" t="s">
+      <c r="G15" s="7"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9">
-      <c r="B16" s="8" t="s">
+      <c r="J15" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="C16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="9">
+      <c r="D16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="9">
-        <v>2</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="9">
+      <c r="G16" s="9"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="3:10">
+      <c r="C17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="9">
         <v>1</v>
       </c>
-      <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="9">
-        <v>2</v>
-      </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="9">
+      <c r="G17" s="9"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="3:10">
+      <c r="C18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="9">
         <v>1</v>
       </c>
-      <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="9">
+      <c r="G18" s="9"/>
+      <c r="H18" s="19">
         <v>3</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="9">
-        <v>1</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9">
-        <v>3</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="B20" s="8" t="s">
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="3:10">
+      <c r="C19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="9">
-        <v>1</v>
-      </c>
-      <c r="D20" s="9"/>
+    </row>
+    <row r="20" spans="3:10">
+      <c r="C20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="9">
+        <v>6</v>
+      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="9">
-        <v>3</v>
-      </c>
-      <c r="H20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="2:9">
-      <c r="B21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="9">
-        <v>1</v>
-      </c>
-      <c r="D21" s="9"/>
+      <c r="J20" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10">
+      <c r="C21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="9">
+        <v>2</v>
+      </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="9">
-        <v>3</v>
-      </c>
-      <c r="H21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="2:9">
-      <c r="B22" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="9">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="3:10">
+      <c r="C22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="9">
+        <v>2</v>
+      </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="9">
-        <v>3</v>
-      </c>
-      <c r="H22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="2:9">
-      <c r="B23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="9">
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="3:10">
+      <c r="C23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="9">
         <v>1</v>
       </c>
-      <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="9">
-        <v>3</v>
-      </c>
-      <c r="H23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="2:9">
-      <c r="B24" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="9">
-        <v>1</v>
-      </c>
-      <c r="D24" s="9"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="3:10">
+      <c r="C24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="9">
+        <v>6</v>
+      </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="9">
+      <c r="G24" s="9"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="3:10">
+      <c r="C25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="9">
         <v>3</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="2:9">
-      <c r="B25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="7">
-        <v>4</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7">
-        <v>3</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9">
-      <c r="B26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="9">
-        <v>6</v>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="3:10">
+      <c r="C26" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="9">
-        <v>4</v>
-      </c>
-      <c r="H26" s="9"/>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="2:9">
-      <c r="B27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="9">
-        <v>6</v>
+      <c r="G26" s="9"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="3:10">
+      <c r="C27" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="9">
-        <v>4</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="2:9">
-      <c r="B28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="3:10">
+      <c r="C28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4">
+        <v>2</v>
+      </c>
       <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="2:9">
-      <c r="B29" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="3:10">
+      <c r="C29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="4">
+        <v>6</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4">
+        <v>2</v>
+      </c>
       <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="2:9">
-      <c r="B30" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="3:10">
+      <c r="C30" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4">
-        <v>2</v>
-      </c>
-      <c r="H30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4">
+        <v>2</v>
+      </c>
       <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="2:9">
-      <c r="B31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="4">
-        <v>6</v>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="3:10">
+      <c r="C31" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="4">
-        <v>2</v>
-      </c>
-      <c r="H31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4">
+        <v>2</v>
+      </c>
       <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="2:9">
-      <c r="B32" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="4"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="3:10">
+      <c r="C32" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4">
-        <v>2</v>
-      </c>
-      <c r="H32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4">
+        <v>2</v>
+      </c>
       <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="2:9">
-      <c r="B33" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="3:10">
+      <c r="C33" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="5"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4">
-        <v>2</v>
-      </c>
-      <c r="H33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4">
+        <v>3</v>
+      </c>
       <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="2:9">
-      <c r="B34" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="4"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="3:10">
+      <c r="C34" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4">
-        <v>2</v>
-      </c>
-      <c r="H34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4">
+        <v>3</v>
+      </c>
       <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="2:9">
-      <c r="B35" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="5"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="3:10">
+      <c r="C35" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4">
+      <c r="G35" s="4"/>
+      <c r="H35" s="4">
         <v>3</v>
       </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="2:9">
-      <c r="B36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="3:10">
+      <c r="C36" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="5"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="4">
+      <c r="G36" s="4"/>
+      <c r="H36" s="4">
         <v>3</v>
       </c>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="2:9">
-      <c r="B37" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="4"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="3:10">
+      <c r="C37" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="4">
+      <c r="G37" s="4"/>
+      <c r="H37" s="4">
         <v>3</v>
       </c>
-      <c r="H37" s="3"/>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="2:9">
-      <c r="B38" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="3:10">
+      <c r="C38" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="5"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="4">
+      <c r="G38" s="4"/>
+      <c r="H38" s="4">
         <v>3</v>
       </c>
-      <c r="H38" s="3"/>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="2:9">
-      <c r="B39" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="4"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="3:10">
+      <c r="C39" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="4">
+      <c r="G39" s="4"/>
+      <c r="H39" s="4">
         <v>3</v>
       </c>
-      <c r="H39" s="3"/>
-      <c r="I39" s="4"/>
-    </row>
-    <row r="40" spans="2:9">
-      <c r="B40" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="5"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="3:10">
+      <c r="C40" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="4">
+      <c r="G40" s="4"/>
+      <c r="H40" s="4">
         <v>3</v>
       </c>
-      <c r="H40" s="3"/>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="41" spans="2:9">
-      <c r="B41" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="4"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="3:10">
+      <c r="C41" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="4">
+      <c r="G41" s="4"/>
+      <c r="H41" s="4">
         <v>3</v>
       </c>
-      <c r="H41" s="3"/>
-      <c r="I41" s="4"/>
-    </row>
-    <row r="42" spans="2:9">
-      <c r="B42" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="4"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="3:10">
+      <c r="C42" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="4">
+      <c r="G42" s="4"/>
+      <c r="H42" s="4">
         <v>3</v>
       </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="4"/>
-    </row>
-    <row r="43" spans="2:9">
-      <c r="B43" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="3:10">
+      <c r="C43" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="4">
+      <c r="G43" s="4"/>
+      <c r="H43" s="4">
         <v>3</v>
       </c>
-      <c r="H43" s="3"/>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="2:9">
-      <c r="B44" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="4"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="3:10">
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="4">
+      <c r="G44" s="4"/>
+      <c r="H44" s="4">
         <v>3</v>
       </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="2:9">
-      <c r="B45" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="5"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="3:10">
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="4">
+      <c r="G45" s="4"/>
+      <c r="H45" s="4">
         <v>3</v>
       </c>
-      <c r="H45" s="3"/>
-      <c r="I45" s="4"/>
-    </row>
-    <row r="46" spans="2:9">
-      <c r="C46" s="4"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="3:10">
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="4">
+      <c r="G46" s="4"/>
+      <c r="H46" s="4">
         <v>3</v>
       </c>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="2:9">
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4">
-        <v>3</v>
-      </c>
-      <c r="H47" s="3"/>
-    </row>
-    <row r="48" spans="2:9">
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4">
-        <v>3</v>
-      </c>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="8"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="H9:H17"/>
+    <mergeCell ref="H18:H23"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Actualizacion completa de calendario hasta la quinta semana
</commit_message>
<xml_diff>
--- a/documentos/General/CronogramaTSP.xlsx
+++ b/documentos/General/CronogramaTSP.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t>Tarea</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Implementación en Servidor</t>
+  </si>
+  <si>
+    <t>Manual de Usuario</t>
   </si>
 </sst>
 </file>
@@ -538,12 +541,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -553,6 +550,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="239">
@@ -1125,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1146,35 +1149,35 @@
     <row r="2" spans="1:10">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6">
@@ -1185,14 +1188,14 @@
         <v>2</v>
       </c>
       <c r="F3" s="6">
-        <f>D3*100/$E$43</f>
-        <v>1.7094017094017093</v>
+        <f>D3*100/$E$44</f>
+        <v>1.6260162601626016</v>
       </c>
       <c r="G3" s="6">
         <f>F3</f>
-        <v>1.7094017094017093</v>
-      </c>
-      <c r="H3" s="7">
+        <v>1.6260162601626016</v>
+      </c>
+      <c r="H3" s="12">
         <v>1</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -1205,7 +1208,7 @@
     <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="6">
@@ -1216,14 +1219,14 @@
         <v>6</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" ref="F4:F43" si="0">D4*100/$E$43</f>
-        <v>3.4188034188034186</v>
+        <f>D4*100/$E$44</f>
+        <v>3.2520325203252032</v>
       </c>
       <c r="G4" s="6">
         <f>F4+G3</f>
-        <v>5.1282051282051277</v>
-      </c>
-      <c r="H4" s="7"/>
+        <v>4.8780487804878048</v>
+      </c>
+      <c r="H4" s="12"/>
       <c r="I4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1234,25 +1237,25 @@
     <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6">
         <v>4</v>
       </c>
       <c r="E5" s="6">
-        <f t="shared" ref="E5:E43" si="1">E4+D5</f>
+        <f t="shared" ref="E5:E44" si="0">E4+D5</f>
         <v>10</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="0"/>
-        <v>3.4188034188034186</v>
+        <f t="shared" ref="F5:F44" si="1">D5*100/$E$44</f>
+        <v>3.2520325203252032</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" ref="G5:G43" si="2">F5+G4</f>
-        <v>8.5470085470085468</v>
-      </c>
-      <c r="H5" s="7"/>
+        <f t="shared" ref="G5:G44" si="2">F5+G4</f>
+        <v>8.1300813008130071</v>
+      </c>
+      <c r="H5" s="12"/>
       <c r="I5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1263,25 +1266,25 @@
     <row r="6" spans="1:10">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
       </c>
       <c r="E6" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" si="2"/>
-        <v>9.4017094017094021</v>
-      </c>
-      <c r="H6" s="7"/>
+        <v>8.9430894308943074</v>
+      </c>
+      <c r="H6" s="12"/>
       <c r="I6" s="6" t="s">
         <v>11</v>
       </c>
@@ -1292,25 +1295,25 @@
     <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
       </c>
       <c r="E7" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F7" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="2"/>
-        <v>10.256410256410257</v>
-      </c>
-      <c r="H7" s="7"/>
+        <v>9.7560975609756078</v>
+      </c>
+      <c r="H7" s="12"/>
       <c r="I7" s="6" t="s">
         <v>11</v>
       </c>
@@ -1321,25 +1324,25 @@
     <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G8" s="6">
         <f t="shared" si="2"/>
-        <v>11.111111111111112</v>
-      </c>
-      <c r="H8" s="7"/>
+        <v>10.569105691056908</v>
+      </c>
+      <c r="H8" s="12"/>
       <c r="I8" s="6" t="s">
         <v>11</v>
       </c>
@@ -1350,25 +1353,25 @@
     <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
       </c>
       <c r="E9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G9" s="6">
         <f t="shared" si="2"/>
-        <v>11.965811965811968</v>
-      </c>
-      <c r="H9" s="7"/>
+        <v>11.382113821138208</v>
+      </c>
+      <c r="H9" s="12"/>
       <c r="I9" s="6" t="s">
         <v>11</v>
       </c>
@@ -1379,25 +1382,25 @@
     <row r="10" spans="1:10">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G10" s="6">
         <f t="shared" si="2"/>
-        <v>12.820512820512823</v>
-      </c>
-      <c r="H10" s="7"/>
+        <v>12.195121951219509</v>
+      </c>
+      <c r="H10" s="12"/>
       <c r="I10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1408,25 +1411,25 @@
     <row r="11" spans="1:10">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="6">
         <v>2</v>
       </c>
       <c r="E11" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" si="0"/>
-        <v>1.7094017094017093</v>
+        <f t="shared" si="1"/>
+        <v>1.6260162601626016</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" si="2"/>
-        <v>14.529914529914532</v>
-      </c>
-      <c r="H11" s="8">
+        <v>13.82113821138211</v>
+      </c>
+      <c r="H11" s="11">
         <v>2</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -1439,25 +1442,25 @@
     <row r="12" spans="1:10">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="5">
         <v>3</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="F12" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5641025641025643</v>
+      <c r="F12" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4390243902439024</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="2"/>
-        <v>17.094017094017097</v>
-      </c>
-      <c r="H12" s="8"/>
+        <v>16.260162601626011</v>
+      </c>
+      <c r="H12" s="11"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5" t="s">
         <v>22</v>
@@ -1466,25 +1469,25 @@
     <row r="13" spans="1:10">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="F13" s="5">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+      <c r="F13" s="6">
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="2"/>
-        <v>17.948717948717952</v>
-      </c>
-      <c r="H13" s="8"/>
+        <v>17.073170731707311</v>
+      </c>
+      <c r="H13" s="11"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5" t="s">
         <v>21</v>
@@ -1493,25 +1496,25 @@
     <row r="14" spans="1:10">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="F14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+      <c r="F14" s="6">
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="2"/>
-        <v>18.803418803418808</v>
-      </c>
-      <c r="H14" s="8"/>
+        <v>17.886178861788611</v>
+      </c>
+      <c r="H14" s="11"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5" t="s">
         <v>19</v>
@@ -1520,25 +1523,25 @@
     <row r="15" spans="1:10">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="5">
         <v>8</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="F15" s="5">
-        <f t="shared" si="0"/>
-        <v>6.8376068376068373</v>
+      <c r="F15" s="6">
+        <f t="shared" si="1"/>
+        <v>6.5040650406504064</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="2"/>
-        <v>25.641025641025646</v>
-      </c>
-      <c r="H15" s="8"/>
+        <v>24.390243902439018</v>
+      </c>
+      <c r="H15" s="11"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5" t="s">
         <v>19</v>
@@ -1547,25 +1550,25 @@
     <row r="16" spans="1:10">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="5">
         <v>3</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="F16" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5641025641025643</v>
+      <c r="F16" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4390243902439024</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="2"/>
-        <v>28.205128205128212</v>
-      </c>
-      <c r="H16" s="8">
+        <v>26.829268292682919</v>
+      </c>
+      <c r="H16" s="11">
         <v>3</v>
       </c>
       <c r="I16" s="5"/>
@@ -1574,25 +1577,25 @@
       </c>
     </row>
     <row r="17" spans="3:10">
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G17" s="6">
         <f t="shared" si="2"/>
-        <v>29.059829059829067</v>
-      </c>
-      <c r="H17" s="8"/>
+        <v>27.642276422764219</v>
+      </c>
+      <c r="H17" s="11"/>
       <c r="I17" s="6" t="s">
         <v>11</v>
       </c>
@@ -1601,25 +1604,25 @@
       </c>
     </row>
     <row r="18" spans="3:10">
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
       </c>
       <c r="E18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="F18" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" si="2"/>
-        <v>29.914529914529922</v>
-      </c>
-      <c r="H18" s="8"/>
+        <v>28.455284552845519</v>
+      </c>
+      <c r="H18" s="11"/>
       <c r="I18" s="6" t="s">
         <v>11</v>
       </c>
@@ -1628,25 +1631,25 @@
       </c>
     </row>
     <row r="19" spans="3:10">
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
       </c>
       <c r="E19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" si="2"/>
-        <v>30.769230769230777</v>
-      </c>
-      <c r="H19" s="8"/>
+        <v>29.26829268292682</v>
+      </c>
+      <c r="H19" s="11"/>
       <c r="I19" s="6" t="s">
         <v>11</v>
       </c>
@@ -1655,25 +1658,25 @@
       </c>
     </row>
     <row r="20" spans="3:10">
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="F20" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G20" s="6">
         <f t="shared" si="2"/>
-        <v>31.623931623931632</v>
-      </c>
-      <c r="H20" s="8"/>
+        <v>30.08130081300812</v>
+      </c>
+      <c r="H20" s="11"/>
       <c r="I20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1682,25 +1685,25 @@
       </c>
     </row>
     <row r="21" spans="3:10">
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
       <c r="E21" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="F21" s="6">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G21" s="6">
         <f t="shared" si="2"/>
-        <v>32.478632478632484</v>
-      </c>
-      <c r="H21" s="8"/>
+        <v>30.89430894308942</v>
+      </c>
+      <c r="H21" s="11"/>
       <c r="I21" s="6" t="s">
         <v>11</v>
       </c>
@@ -1709,75 +1712,75 @@
       </c>
     </row>
     <row r="22" spans="3:10">
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="5">
         <v>4</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="F22" s="5">
-        <f t="shared" si="0"/>
-        <v>3.4188034188034186</v>
+      <c r="F22" s="6">
+        <f t="shared" si="1"/>
+        <v>3.2520325203252032</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="2"/>
-        <v>35.897435897435905</v>
-      </c>
-      <c r="H22" s="8"/>
+        <v>34.146341463414622</v>
+      </c>
+      <c r="H22" s="11"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="3:10">
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="5">
         <v>3</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="F23" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5641025641025643</v>
+      <c r="F23" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4390243902439024</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="2"/>
-        <v>38.461538461538467</v>
-      </c>
-      <c r="H23" s="8"/>
+        <v>36.585365853658523</v>
+      </c>
+      <c r="H23" s="11"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="3:10">
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D24" s="5">
         <v>3</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="F24" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5641025641025643</v>
+      <c r="F24" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4390243902439024</v>
       </c>
       <c r="G24" s="5">
         <f t="shared" si="2"/>
-        <v>41.025641025641029</v>
-      </c>
-      <c r="H24" s="8">
+        <v>39.024390243902424</v>
+      </c>
+      <c r="H24" s="11">
         <v>4</v>
       </c>
       <c r="I24" s="5"/>
@@ -1786,75 +1789,75 @@
       </c>
     </row>
     <row r="25" spans="3:10">
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="5">
         <v>8</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="F25" s="5">
-        <f t="shared" si="0"/>
-        <v>6.8376068376068373</v>
+      <c r="F25" s="6">
+        <f t="shared" si="1"/>
+        <v>6.5040650406504064</v>
       </c>
       <c r="G25" s="5">
         <f t="shared" si="2"/>
-        <v>47.863247863247864</v>
-      </c>
-      <c r="H25" s="8"/>
+        <v>45.528455284552834</v>
+      </c>
+      <c r="H25" s="11"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="3:10">
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="5">
         <v>3</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="F26" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5641025641025643</v>
+      <c r="F26" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4390243902439024</v>
       </c>
       <c r="G26" s="5">
         <f t="shared" si="2"/>
-        <v>50.427350427350426</v>
-      </c>
-      <c r="H26" s="8"/>
+        <v>47.967479674796735</v>
+      </c>
+      <c r="H26" s="11"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="3:10">
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="6">
         <v>2</v>
       </c>
       <c r="E27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="F27" s="6">
-        <f t="shared" si="0"/>
-        <v>1.7094017094017093</v>
+        <f t="shared" si="1"/>
+        <v>1.6260162601626016</v>
       </c>
       <c r="G27" s="6">
         <f t="shared" si="2"/>
-        <v>52.136752136752136</v>
-      </c>
-      <c r="H27" s="8"/>
+        <v>49.593495934959336</v>
+      </c>
+      <c r="H27" s="11"/>
       <c r="I27" s="6" t="s">
         <v>11</v>
       </c>
@@ -1863,25 +1866,25 @@
       </c>
     </row>
     <row r="28" spans="3:10">
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="6">
         <v>2</v>
       </c>
       <c r="E28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="F28" s="6">
-        <f t="shared" si="0"/>
-        <v>1.7094017094017093</v>
+        <f t="shared" si="1"/>
+        <v>1.6260162601626016</v>
       </c>
       <c r="G28" s="6">
         <f t="shared" si="2"/>
-        <v>53.846153846153847</v>
-      </c>
-      <c r="H28" s="8">
+        <v>51.219512195121936</v>
+      </c>
+      <c r="H28" s="11">
         <v>5</v>
       </c>
       <c r="I28" s="6" t="s">
@@ -1892,25 +1895,25 @@
       </c>
     </row>
     <row r="29" spans="3:10">
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="6">
         <v>2</v>
       </c>
       <c r="E29" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>65</v>
       </c>
       <c r="F29" s="6">
-        <f t="shared" si="0"/>
-        <v>1.7094017094017093</v>
+        <f t="shared" si="1"/>
+        <v>1.6260162601626016</v>
       </c>
       <c r="G29" s="6">
         <f t="shared" si="2"/>
-        <v>55.555555555555557</v>
-      </c>
-      <c r="H29" s="8"/>
+        <v>52.845528455284537</v>
+      </c>
+      <c r="H29" s="11"/>
       <c r="I29" s="6" t="s">
         <v>11</v>
       </c>
@@ -1919,125 +1922,125 @@
       </c>
     </row>
     <row r="30" spans="3:10">
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="5">
         <v>1</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="F30" s="5">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+      <c r="F30" s="6">
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G30" s="5">
         <f t="shared" si="2"/>
-        <v>56.410256410256409</v>
-      </c>
-      <c r="H30" s="8"/>
+        <v>53.658536585365837</v>
+      </c>
+      <c r="H30" s="11"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="31" spans="3:10">
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="5">
         <v>2</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="F31" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7094017094017093</v>
+      <c r="F31" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6260162601626016</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" si="2"/>
-        <v>58.119658119658119</v>
-      </c>
-      <c r="H31" s="8"/>
+        <v>55.284552845528438</v>
+      </c>
+      <c r="H31" s="11"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" spans="3:10">
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="5">
         <v>2</v>
       </c>
       <c r="E32" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="F32" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7094017094017093</v>
+      <c r="F32" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6260162601626016</v>
       </c>
       <c r="G32" s="5">
         <f t="shared" si="2"/>
-        <v>59.82905982905983</v>
-      </c>
-      <c r="H32" s="8"/>
+        <v>56.910569105691039</v>
+      </c>
+      <c r="H32" s="11"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="3:10">
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="5">
         <v>2</v>
       </c>
       <c r="E33" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="F33" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7094017094017093</v>
+      <c r="F33" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6260162601626016</v>
       </c>
       <c r="G33" s="5">
         <f t="shared" si="2"/>
-        <v>61.53846153846154</v>
-      </c>
-      <c r="H33" s="8"/>
+        <v>58.536585365853639</v>
+      </c>
+      <c r="H33" s="11"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="34" spans="3:10">
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="6">
         <v>4</v>
       </c>
       <c r="E34" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="F34" s="6">
-        <f t="shared" si="0"/>
-        <v>3.4188034188034186</v>
+        <f t="shared" si="1"/>
+        <v>3.2520325203252032</v>
       </c>
       <c r="G34" s="6">
         <f t="shared" si="2"/>
-        <v>64.957264957264954</v>
-      </c>
-      <c r="H34" s="8"/>
+        <v>61.788617886178841</v>
+      </c>
+      <c r="H34" s="11"/>
       <c r="I34" s="6" t="s">
         <v>11</v>
       </c>
@@ -2046,227 +2049,242 @@
       </c>
     </row>
     <row r="35" spans="3:10">
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="5">
         <v>6</v>
       </c>
       <c r="E35" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="F35" s="5">
-        <f t="shared" si="0"/>
-        <v>5.1282051282051286</v>
+      <c r="F35" s="6">
+        <f t="shared" si="1"/>
+        <v>4.8780487804878048</v>
       </c>
       <c r="G35" s="5">
         <f t="shared" si="2"/>
-        <v>70.085470085470078</v>
-      </c>
-      <c r="H35" s="8">
+        <v>66.666666666666643</v>
+      </c>
+      <c r="H35" s="11">
         <v>6</v>
       </c>
       <c r="I35" s="5"/>
-      <c r="J35" s="9" t="s">
+      <c r="J35" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="36" spans="3:10">
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="F36" s="5">
-        <f t="shared" si="0"/>
-        <v>0.85470085470085466</v>
+      <c r="F36" s="6">
+        <f t="shared" si="1"/>
+        <v>0.81300813008130079</v>
       </c>
       <c r="G36" s="5">
         <f t="shared" si="2"/>
-        <v>70.94017094017093</v>
-      </c>
-      <c r="H36" s="8"/>
+        <v>67.479674796747943</v>
+      </c>
+      <c r="H36" s="11"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="9"/>
+      <c r="J36" s="7"/>
     </row>
     <row r="37" spans="3:10">
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="9" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="5">
         <v>2</v>
       </c>
       <c r="E37" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="F37" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7094017094017093</v>
+      <c r="F37" s="6">
+        <f t="shared" si="1"/>
+        <v>1.6260162601626016</v>
       </c>
       <c r="G37" s="5">
         <f t="shared" si="2"/>
-        <v>72.649572649572633</v>
-      </c>
-      <c r="H37" s="8"/>
+        <v>69.105691056910544</v>
+      </c>
+      <c r="H37" s="11"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="9"/>
+      <c r="J37" s="7"/>
     </row>
     <row r="38" spans="3:10">
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D38" s="5">
         <v>3</v>
       </c>
       <c r="E38" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="F38" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5641025641025643</v>
+      <c r="F38" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4390243902439024</v>
       </c>
       <c r="G38" s="5">
         <f t="shared" si="2"/>
-        <v>75.213675213675202</v>
-      </c>
-      <c r="H38" s="8"/>
+        <v>71.544715447154445</v>
+      </c>
+      <c r="H38" s="11"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
     <row r="39" spans="3:10">
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="10" t="s">
         <v>51</v>
       </c>
       <c r="D39" s="5">
         <v>3</v>
       </c>
       <c r="E39" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="F39" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5641025641025643</v>
+      <c r="F39" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4390243902439024</v>
       </c>
       <c r="G39" s="5">
         <f t="shared" si="2"/>
-        <v>77.777777777777771</v>
-      </c>
-      <c r="H39" s="8"/>
+        <v>73.983739837398346</v>
+      </c>
+      <c r="H39" s="11"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="3:10">
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D40" s="5">
         <v>10</v>
       </c>
       <c r="E40" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="F40" s="5">
-        <f t="shared" si="0"/>
-        <v>8.5470085470085468</v>
+      <c r="F40" s="6">
+        <f t="shared" si="1"/>
+        <v>8.1300813008130088</v>
       </c>
       <c r="G40" s="5">
         <f t="shared" si="2"/>
-        <v>86.324786324786317</v>
-      </c>
-      <c r="H40" s="8">
+        <v>82.11382113821135</v>
+      </c>
+      <c r="H40" s="11">
         <v>7</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
     <row r="41" spans="3:10">
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D41" s="5">
         <v>6</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="F41" s="5">
-        <f t="shared" si="0"/>
-        <v>5.1282051282051286</v>
+      <c r="F41" s="6">
+        <f t="shared" si="1"/>
+        <v>4.8780487804878048</v>
       </c>
       <c r="G41" s="5">
         <f t="shared" si="2"/>
-        <v>91.452991452991441</v>
-      </c>
-      <c r="H41" s="8"/>
+        <v>86.991869918699152</v>
+      </c>
+      <c r="H41" s="11"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="3:10">
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D42" s="5">
         <v>4</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>111</v>
       </c>
-      <c r="F42" s="5">
-        <f t="shared" si="0"/>
-        <v>3.4188034188034186</v>
+      <c r="F42" s="6">
+        <f t="shared" si="1"/>
+        <v>3.2520325203252032</v>
       </c>
       <c r="G42" s="5">
         <f t="shared" si="2"/>
-        <v>94.871794871794862</v>
-      </c>
-      <c r="H42" s="8">
+        <v>90.243902439024353</v>
+      </c>
+      <c r="H42" s="11">
         <v>8</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="3:10">
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D43" s="5">
         <v>6</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="F43" s="5">
-        <f t="shared" si="0"/>
-        <v>5.1282051282051286</v>
+      <c r="F43" s="6">
+        <f t="shared" si="1"/>
+        <v>4.8780487804878048</v>
       </c>
       <c r="G43" s="5">
         <f t="shared" si="2"/>
-        <v>99.999999999999986</v>
-      </c>
-      <c r="H43" s="8"/>
+        <v>95.121951219512155</v>
+      </c>
+      <c r="H43" s="11"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="3:10">
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="2"/>
+      <c r="C44" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="5">
+        <v>6</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="F44" s="6">
+        <f t="shared" si="1"/>
+        <v>4.8780487804878048</v>
+      </c>
+      <c r="G44" s="5">
+        <f t="shared" si="2"/>
+        <v>99.999999999999957</v>
+      </c>
+      <c r="H44" s="11"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
     </row>
     <row r="45" spans="3:10">
       <c r="D45" s="3"/>
@@ -2290,7 +2308,6 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="H42:H43"/>
     <mergeCell ref="H3:H10"/>
     <mergeCell ref="H11:H15"/>
     <mergeCell ref="H16:H23"/>
@@ -2298,9 +2315,9 @@
     <mergeCell ref="H28:H34"/>
     <mergeCell ref="H35:H39"/>
     <mergeCell ref="H40:H41"/>
+    <mergeCell ref="H42:H44"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
ECU reorganizados, se cambian identificadores para agruparlos por fecha y funcionalidades
</commit_message>
<xml_diff>
--- a/documentos/General/CronogramaTSP.xlsx
+++ b/documentos/General/CronogramaTSP.xlsx
@@ -90,9 +90,6 @@
     <t>Juan Castaño</t>
   </si>
   <si>
-    <t>Juan Esteban</t>
-  </si>
-  <si>
     <t>ECU. Registrar pacientes</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>Manual de Usuario</t>
+  </si>
+  <si>
+    <t>Julian</t>
   </si>
 </sst>
 </file>
@@ -551,10 +551,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1128,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1195,7 +1195,7 @@
         <f>F3</f>
         <v>1.6260162601626016</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="11">
         <v>1</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -1226,7 +1226,7 @@
         <f>F4+G3</f>
         <v>4.8780487804878048</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1255,7 +1255,7 @@
         <f t="shared" ref="G5:G44" si="2">F5+G4</f>
         <v>8.1300813008130071</v>
       </c>
-      <c r="H5" s="12"/>
+      <c r="H5" s="11"/>
       <c r="I5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1284,7 +1284,7 @@
         <f t="shared" si="2"/>
         <v>8.9430894308943074</v>
       </c>
-      <c r="H6" s="12"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="6" t="s">
         <v>11</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="4"/>
       <c r="C7" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -1313,19 +1313,19 @@
         <f t="shared" si="2"/>
         <v>9.7560975609756078</v>
       </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="11"/>
       <c r="I7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="2"/>
       <c r="B8" s="4"/>
       <c r="C8" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
@@ -1342,19 +1342,19 @@
         <f t="shared" si="2"/>
         <v>10.569105691056908</v>
       </c>
-      <c r="H8" s="12"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" s="4"/>
       <c r="C9" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6">
         <v>1</v>
@@ -1371,19 +1371,19 @@
         <f t="shared" si="2"/>
         <v>11.382113821138208</v>
       </c>
-      <c r="H9" s="12"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="2"/>
       <c r="B10" s="4"/>
       <c r="C10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -1400,7 +1400,7 @@
         <f t="shared" si="2"/>
         <v>12.195121951219509</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1412,7 +1412,7 @@
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="6">
         <v>2</v>
@@ -1429,7 +1429,7 @@
         <f t="shared" si="2"/>
         <v>13.82113821138211</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="12">
         <v>2</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -1443,7 +1443,7 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="5">
         <v>3</v>
@@ -1460,7 +1460,7 @@
         <f t="shared" si="2"/>
         <v>16.260162601626011</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5" t="s">
         <v>22</v>
@@ -1470,7 +1470,7 @@
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
@@ -1487,7 +1487,7 @@
         <f t="shared" si="2"/>
         <v>17.073170731707311</v>
       </c>
-      <c r="H13" s="11"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5" t="s">
         <v>21</v>
@@ -1497,7 +1497,7 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
@@ -1514,7 +1514,7 @@
         <f t="shared" si="2"/>
         <v>17.886178861788611</v>
       </c>
-      <c r="H14" s="11"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5" t="s">
         <v>19</v>
@@ -1524,7 +1524,7 @@
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="5">
         <v>8</v>
@@ -1541,7 +1541,7 @@
         <f t="shared" si="2"/>
         <v>24.390243902439018</v>
       </c>
-      <c r="H15" s="11"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5" t="s">
         <v>19</v>
@@ -1551,7 +1551,7 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="5">
         <v>3</v>
@@ -1568,7 +1568,7 @@
         <f t="shared" si="2"/>
         <v>26.829268292682919</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="12">
         <v>3</v>
       </c>
       <c r="I16" s="5"/>
@@ -1595,7 +1595,7 @@
         <f t="shared" si="2"/>
         <v>27.642276422764219</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="6" t="s">
         <v>11</v>
       </c>
@@ -1622,7 +1622,7 @@
         <f t="shared" si="2"/>
         <v>28.455284552845519</v>
       </c>
-      <c r="H18" s="11"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="6" t="s">
         <v>11</v>
       </c>
@@ -1649,7 +1649,7 @@
         <f t="shared" si="2"/>
         <v>29.26829268292682</v>
       </c>
-      <c r="H19" s="11"/>
+      <c r="H19" s="12"/>
       <c r="I19" s="6" t="s">
         <v>11</v>
       </c>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="20" spans="3:10">
       <c r="C20" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
@@ -1676,7 +1676,7 @@
         <f t="shared" si="2"/>
         <v>30.08130081300812</v>
       </c>
-      <c r="H20" s="11"/>
+      <c r="H20" s="12"/>
       <c r="I20" s="6" t="s">
         <v>11</v>
       </c>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="21" spans="3:10">
       <c r="C21" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -1703,7 +1703,7 @@
         <f t="shared" si="2"/>
         <v>30.89430894308942</v>
       </c>
-      <c r="H21" s="11"/>
+      <c r="H21" s="12"/>
       <c r="I21" s="6" t="s">
         <v>11</v>
       </c>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="22" spans="3:10">
       <c r="C22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="5">
         <v>4</v>
@@ -1730,7 +1730,7 @@
         <f t="shared" si="2"/>
         <v>34.146341463414622</v>
       </c>
-      <c r="H22" s="11"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
         <v>22</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="23" spans="3:10">
       <c r="C23" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D23" s="5">
         <v>3</v>
@@ -1755,7 +1755,7 @@
         <f t="shared" si="2"/>
         <v>36.585365853658523</v>
       </c>
-      <c r="H23" s="11"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5" t="s">
         <v>19</v>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="24" spans="3:10">
       <c r="C24" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="5">
         <v>3</v>
@@ -1780,7 +1780,7 @@
         <f t="shared" si="2"/>
         <v>39.024390243902424</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="12">
         <v>4</v>
       </c>
       <c r="I24" s="5"/>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="25" spans="3:10">
       <c r="C25" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="5">
         <v>8</v>
@@ -1807,7 +1807,7 @@
         <f t="shared" si="2"/>
         <v>45.528455284552834</v>
       </c>
-      <c r="H25" s="11"/>
+      <c r="H25" s="12"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5" t="s">
         <v>19</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="26" spans="3:10">
       <c r="C26" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5">
         <v>3</v>
@@ -1832,7 +1832,7 @@
         <f t="shared" si="2"/>
         <v>47.967479674796735</v>
       </c>
-      <c r="H26" s="11"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5" t="s">
         <v>21</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="27" spans="3:10">
       <c r="C27" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="6">
         <v>2</v>
@@ -1857,7 +1857,7 @@
         <f t="shared" si="2"/>
         <v>49.593495934959336</v>
       </c>
-      <c r="H27" s="11"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="6" t="s">
         <v>11</v>
       </c>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="28" spans="3:10">
       <c r="C28" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="6">
         <v>2</v>
@@ -1884,7 +1884,7 @@
         <f t="shared" si="2"/>
         <v>51.219512195121936</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H28" s="12">
         <v>5</v>
       </c>
       <c r="I28" s="6" t="s">
@@ -1896,7 +1896,7 @@
     </row>
     <row r="29" spans="3:10">
       <c r="C29" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="6">
         <v>2</v>
@@ -1913,7 +1913,7 @@
         <f t="shared" si="2"/>
         <v>52.845528455284537</v>
       </c>
-      <c r="H29" s="11"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="6" t="s">
         <v>11</v>
       </c>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="30" spans="3:10">
       <c r="C30" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30" s="5">
         <v>1</v>
@@ -1940,7 +1940,7 @@
         <f t="shared" si="2"/>
         <v>53.658536585365837</v>
       </c>
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5" t="s">
         <v>20</v>
@@ -1965,7 +1965,7 @@
         <f t="shared" si="2"/>
         <v>55.284552845528438</v>
       </c>
-      <c r="H31" s="11"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5" t="s">
         <v>22</v>
@@ -1990,7 +1990,7 @@
         <f t="shared" si="2"/>
         <v>56.910569105691039</v>
       </c>
-      <c r="H32" s="11"/>
+      <c r="H32" s="12"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5" t="s">
         <v>22</v>
@@ -2015,7 +2015,7 @@
         <f t="shared" si="2"/>
         <v>58.536585365853639</v>
       </c>
-      <c r="H33" s="11"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5" t="s">
         <v>22</v>
@@ -2023,7 +2023,7 @@
     </row>
     <row r="34" spans="3:10">
       <c r="C34" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D34" s="6">
         <v>4</v>
@@ -2040,7 +2040,7 @@
         <f t="shared" si="2"/>
         <v>61.788617886178841</v>
       </c>
-      <c r="H34" s="11"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="6" t="s">
         <v>11</v>
       </c>
@@ -2050,7 +2050,7 @@
     </row>
     <row r="35" spans="3:10">
       <c r="C35" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D35" s="5">
         <v>6</v>
@@ -2067,7 +2067,7 @@
         <f t="shared" si="2"/>
         <v>66.666666666666643</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="12">
         <v>6</v>
       </c>
       <c r="I35" s="5"/>
@@ -2077,7 +2077,7 @@
     </row>
     <row r="36" spans="3:10">
       <c r="C36" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
@@ -2094,13 +2094,13 @@
         <f t="shared" si="2"/>
         <v>67.479674796747943</v>
       </c>
-      <c r="H36" s="11"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="5"/>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="3:10">
       <c r="C37" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="5">
         <v>2</v>
@@ -2117,13 +2117,13 @@
         <f t="shared" si="2"/>
         <v>69.105691056910544</v>
       </c>
-      <c r="H37" s="11"/>
+      <c r="H37" s="12"/>
       <c r="I37" s="5"/>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="3:10">
       <c r="C38" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" s="5">
         <v>3</v>
@@ -2140,13 +2140,13 @@
         <f t="shared" si="2"/>
         <v>71.544715447154445</v>
       </c>
-      <c r="H38" s="11"/>
+      <c r="H38" s="12"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
     <row r="39" spans="3:10">
       <c r="C39" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" s="5">
         <v>3</v>
@@ -2163,13 +2163,13 @@
         <f t="shared" si="2"/>
         <v>73.983739837398346</v>
       </c>
-      <c r="H39" s="11"/>
+      <c r="H39" s="12"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="3:10">
       <c r="C40" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" s="5">
         <v>10</v>
@@ -2186,7 +2186,7 @@
         <f t="shared" si="2"/>
         <v>82.11382113821135</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H40" s="12">
         <v>7</v>
       </c>
       <c r="I40" s="5"/>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="41" spans="3:10">
       <c r="C41" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="5">
         <v>6</v>
@@ -2211,13 +2211,13 @@
         <f t="shared" si="2"/>
         <v>86.991869918699152</v>
       </c>
-      <c r="H41" s="11"/>
+      <c r="H41" s="12"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="3:10">
       <c r="C42" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42" s="5">
         <v>4</v>
@@ -2234,7 +2234,7 @@
         <f t="shared" si="2"/>
         <v>90.243902439024353</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H42" s="12">
         <v>8</v>
       </c>
       <c r="I42" s="5"/>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="43" spans="3:10">
       <c r="C43" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" s="5">
         <v>6</v>
@@ -2259,13 +2259,13 @@
         <f t="shared" si="2"/>
         <v>95.121951219512155</v>
       </c>
-      <c r="H43" s="11"/>
+      <c r="H43" s="12"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="3:10">
       <c r="C44" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D44" s="5">
         <v>6</v>
@@ -2282,7 +2282,7 @@
         <f t="shared" si="2"/>
         <v>99.999999999999957</v>
       </c>
-      <c r="H44" s="11"/>
+      <c r="H44" s="12"/>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
@@ -2308,14 +2308,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="H42:H44"/>
     <mergeCell ref="H3:H10"/>
     <mergeCell ref="H11:H15"/>
     <mergeCell ref="H16:H23"/>
     <mergeCell ref="H24:H27"/>
     <mergeCell ref="H28:H34"/>
-    <mergeCell ref="H35:H39"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="H42:H44"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Se agrega quinta semana al calendario
</commit_message>
<xml_diff>
--- a/documentos/General/CronogramaTSP.xlsx
+++ b/documentos/General/CronogramaTSP.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="260" windowWidth="25040" windowHeight="14920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="460" yWindow="260" windowWidth="25040" windowHeight="14920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma General" sheetId="1" r:id="rId1"/>
     <sheet name="Cuarta Semana" sheetId="3" r:id="rId2"/>
+    <sheet name="Quinta Semana" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="72">
   <si>
     <t>Tarea</t>
   </si>
@@ -230,6 +231,12 @@
   </si>
   <si>
     <t>Juan Camilo</t>
+  </si>
+  <si>
+    <t>Diseño de clases - Historial médico</t>
+  </si>
+  <si>
+    <t>Diseño de clases - Autentificación de usuarios</t>
   </si>
 </sst>
 </file>
@@ -389,8 +396,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="263">
+  <cellStyleXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -687,19 +704,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="263">
+  <cellStyles count="273">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -831,6 +848,11 @@
     <cellStyle name="Hipervínculo" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="271" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -962,6 +984,11 @@
     <cellStyle name="Hipervínculo visitado" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="272" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1293,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1357,7 +1384,7 @@
         <f>E3</f>
         <v>1.6260162601626016</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="18">
         <v>1</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -1392,7 +1419,7 @@
         <f>E4+F3</f>
         <v>4.8780487804878048</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="5" t="s">
         <v>11</v>
       </c>
@@ -1427,7 +1454,7 @@
         <f t="shared" ref="F5:F44" si="2">E5+F4</f>
         <v>8.1300813008130071</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1454,7 +1481,7 @@
         <f t="shared" si="2"/>
         <v>8.9430894308943074</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1481,7 +1508,7 @@
         <f t="shared" si="2"/>
         <v>9.7560975609756078</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1508,7 +1535,7 @@
         <f t="shared" si="2"/>
         <v>10.569105691056908</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="18"/>
       <c r="H8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1535,7 +1562,7 @@
         <f t="shared" si="2"/>
         <v>11.382113821138208</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1562,7 +1589,7 @@
         <f t="shared" si="2"/>
         <v>12.195121951219509</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1589,7 +1616,7 @@
         <f t="shared" si="2"/>
         <v>13.82113821138211</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="18">
         <v>2</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -1618,7 +1645,7 @@
         <f t="shared" si="2"/>
         <v>16.260162601626011</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1645,7 +1672,7 @@
         <f t="shared" si="2"/>
         <v>17.073170731707311</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1672,7 +1699,7 @@
         <f t="shared" si="2"/>
         <v>17.886178861788611</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1699,7 +1726,7 @@
         <f t="shared" si="2"/>
         <v>24.390243902439018</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="5" t="s">
         <v>11</v>
       </c>
@@ -1727,7 +1754,7 @@
         <f t="shared" si="2"/>
         <v>26.829268292682919</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="18">
         <v>3</v>
       </c>
       <c r="H16" s="13" t="s">
@@ -1756,7 +1783,7 @@
         <f t="shared" si="2"/>
         <v>27.642276422764219</v>
       </c>
-      <c r="G17" s="15"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="5" t="s">
         <v>11</v>
       </c>
@@ -1783,7 +1810,7 @@
         <f t="shared" si="2"/>
         <v>28.455284552845519</v>
       </c>
-      <c r="G18" s="15"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1810,7 +1837,7 @@
         <f t="shared" si="2"/>
         <v>29.26829268292682</v>
       </c>
-      <c r="G19" s="15"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1837,7 +1864,7 @@
         <f t="shared" si="2"/>
         <v>30.08130081300812</v>
       </c>
-      <c r="G20" s="15"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="5" t="s">
         <v>11</v>
       </c>
@@ -1864,7 +1891,7 @@
         <f t="shared" si="2"/>
         <v>30.89430894308942</v>
       </c>
-      <c r="G21" s="15"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1891,7 +1918,7 @@
         <f t="shared" si="2"/>
         <v>34.146341463414622</v>
       </c>
-      <c r="G22" s="15"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="5" t="s">
         <v>11</v>
       </c>
@@ -1918,7 +1945,7 @@
         <f t="shared" si="2"/>
         <v>36.585365853658523</v>
       </c>
-      <c r="G23" s="15"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="5" t="s">
         <v>11</v>
       </c>
@@ -1945,7 +1972,7 @@
         <f t="shared" si="2"/>
         <v>39.024390243902424</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="17">
         <v>4</v>
       </c>
       <c r="H24" s="4" t="s">
@@ -1974,7 +2001,7 @@
         <f t="shared" si="2"/>
         <v>45.528455284552834</v>
       </c>
-      <c r="G25" s="14"/>
+      <c r="G25" s="17"/>
       <c r="H25" s="4" t="s">
         <v>56</v>
       </c>
@@ -2001,7 +2028,7 @@
         <f t="shared" si="2"/>
         <v>47.967479674796735</v>
       </c>
-      <c r="G26" s="14"/>
+      <c r="G26" s="17"/>
       <c r="H26" s="4" t="s">
         <v>56</v>
       </c>
@@ -2028,7 +2055,7 @@
         <f t="shared" si="2"/>
         <v>49.593495934959336</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="17"/>
       <c r="H27" s="5" t="s">
         <v>11</v>
       </c>
@@ -2055,7 +2082,7 @@
         <f t="shared" si="2"/>
         <v>51.219512195121936</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="17">
         <v>5</v>
       </c>
       <c r="H28" s="5" t="s">
@@ -2084,7 +2111,7 @@
         <f t="shared" si="2"/>
         <v>52.845528455284537</v>
       </c>
-      <c r="G29" s="14"/>
+      <c r="G29" s="17"/>
       <c r="H29" s="5" t="s">
         <v>11</v>
       </c>
@@ -2111,7 +2138,7 @@
         <f t="shared" si="2"/>
         <v>53.658536585365837</v>
       </c>
-      <c r="G30" s="14"/>
+      <c r="G30" s="17"/>
       <c r="H30" s="4" t="s">
         <v>56</v>
       </c>
@@ -2138,7 +2165,7 @@
         <f t="shared" si="2"/>
         <v>55.284552845528438</v>
       </c>
-      <c r="G31" s="14"/>
+      <c r="G31" s="17"/>
       <c r="H31" s="4" t="s">
         <v>56</v>
       </c>
@@ -2165,7 +2192,7 @@
         <f t="shared" si="2"/>
         <v>56.910569105691039</v>
       </c>
-      <c r="G32" s="14"/>
+      <c r="G32" s="17"/>
       <c r="H32" s="4" t="s">
         <v>56</v>
       </c>
@@ -2192,7 +2219,7 @@
         <f t="shared" si="2"/>
         <v>58.536585365853639</v>
       </c>
-      <c r="G33" s="14"/>
+      <c r="G33" s="17"/>
       <c r="H33" s="4" t="s">
         <v>56</v>
       </c>
@@ -2219,7 +2246,7 @@
         <f t="shared" si="2"/>
         <v>61.788617886178841</v>
       </c>
-      <c r="G34" s="14"/>
+      <c r="G34" s="17"/>
       <c r="H34" s="5" t="s">
         <v>11</v>
       </c>
@@ -2246,7 +2273,7 @@
         <f t="shared" si="2"/>
         <v>66.666666666666643</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="17">
         <v>6</v>
       </c>
       <c r="H35" s="4" t="s">
@@ -2275,7 +2302,7 @@
         <f t="shared" si="2"/>
         <v>67.479674796747943</v>
       </c>
-      <c r="G36" s="14"/>
+      <c r="G36" s="17"/>
       <c r="H36" s="4" t="s">
         <v>56</v>
       </c>
@@ -2302,7 +2329,7 @@
         <f t="shared" si="2"/>
         <v>69.105691056910544</v>
       </c>
-      <c r="G37" s="14"/>
+      <c r="G37" s="17"/>
       <c r="H37" s="4" t="s">
         <v>56</v>
       </c>
@@ -2329,7 +2356,7 @@
         <f t="shared" si="2"/>
         <v>71.544715447154445</v>
       </c>
-      <c r="G38" s="14"/>
+      <c r="G38" s="17"/>
       <c r="H38" s="4" t="s">
         <v>56</v>
       </c>
@@ -2356,7 +2383,7 @@
         <f t="shared" si="2"/>
         <v>73.983739837398346</v>
       </c>
-      <c r="G39" s="14"/>
+      <c r="G39" s="17"/>
       <c r="H39" s="4" t="s">
         <v>56</v>
       </c>
@@ -2383,7 +2410,7 @@
         <f t="shared" si="2"/>
         <v>82.11382113821135</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="17">
         <v>7</v>
       </c>
       <c r="H40" s="4" t="s">
@@ -2412,7 +2439,7 @@
         <f t="shared" si="2"/>
         <v>86.991869918699152</v>
       </c>
-      <c r="G41" s="14"/>
+      <c r="G41" s="17"/>
       <c r="H41" s="4" t="s">
         <v>56</v>
       </c>
@@ -2439,7 +2466,7 @@
         <f t="shared" si="2"/>
         <v>90.243902439024353</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="17">
         <v>8</v>
       </c>
       <c r="H42" s="4" t="s">
@@ -2468,7 +2495,7 @@
         <f t="shared" si="2"/>
         <v>95.121951219512155</v>
       </c>
-      <c r="G43" s="14"/>
+      <c r="G43" s="17"/>
       <c r="H43" s="4" t="s">
         <v>56</v>
       </c>
@@ -2495,7 +2522,7 @@
         <f t="shared" si="2"/>
         <v>99.999999999999957</v>
       </c>
-      <c r="G44" s="14"/>
+      <c r="G44" s="17"/>
       <c r="H44" s="4" t="s">
         <v>56</v>
       </c>
@@ -2548,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2570,112 +2597,112 @@
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>1</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>1</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>2</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="16">
         <v>3</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="16">
         <v>2</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="16">
         <v>1</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="16">
         <v>1</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="16">
         <v>1</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="16">
         <v>3</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2688,4 +2715,128 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4">
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Organizacion calendario general y definitivo
</commit_message>
<xml_diff>
--- a/documentos/General/CronogramaTSP.xlsx
+++ b/documentos/General/CronogramaTSP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="260" windowWidth="25040" windowHeight="14920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="460" yWindow="260" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma General" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="78">
   <si>
     <t>Tarea</t>
   </si>
@@ -122,12 +122,6 @@
     <t>Diseño de pruebas - Tercera Semana</t>
   </si>
   <si>
-    <t>Creación y configuración de instaladores</t>
-  </si>
-  <si>
-    <t>Prueba Alpha - Priemera version</t>
-  </si>
-  <si>
     <t>Contratos de métodos - Primera Semana</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>Diseño de clases - Primera Semana</t>
   </si>
   <si>
-    <t>Integración de codificación</t>
-  </si>
-  <si>
     <t>Actualización Base de Datos</t>
   </si>
   <si>
@@ -155,36 +146,12 @@
     <t>Diseño de clases - Tercera Semana</t>
   </si>
   <si>
-    <t>Contratos de métodos - Tercera Semana</t>
-  </si>
-  <si>
-    <t>Codificación - Tercera Semana</t>
-  </si>
-  <si>
-    <t>Diseño de pruebas - Cuarta/Quinta Semana</t>
-  </si>
-  <si>
-    <t>Listas de chequeo - ECU Cuarta/Quinta Semana</t>
-  </si>
-  <si>
-    <t>Diseño de clases - Cuarta/Quinta Semana</t>
-  </si>
-  <si>
-    <t>Junit - Cuarta/Quinta Semana</t>
-  </si>
-  <si>
-    <t>Implementación en Servidor</t>
-  </si>
-  <si>
     <t>Manual de Usuario</t>
   </si>
   <si>
     <t>Julian</t>
   </si>
   <si>
-    <t>NN</t>
-  </si>
-  <si>
     <t>Completado</t>
   </si>
   <si>
@@ -194,15 +161,9 @@
     <t>-</t>
   </si>
   <si>
-    <t>Juan Esteban</t>
-  </si>
-  <si>
     <t>Jenny y Julián</t>
   </si>
   <si>
-    <t>Junit - Tercera semana</t>
-  </si>
-  <si>
     <t>Contrato - Modificar propietario</t>
   </si>
   <si>
@@ -237,13 +198,70 @@
   </si>
   <si>
     <t>Diseño de clases - Autentificación de usuarios</t>
+  </si>
+  <si>
+    <t>Listas de chequeo - ECU Cuarta y Quinta Semana</t>
+  </si>
+  <si>
+    <t>Contrato - Registrar historial médico</t>
+  </si>
+  <si>
+    <t>Contrato - Consultar historial médico</t>
+  </si>
+  <si>
+    <t>Contrato - Modificar historial médico</t>
+  </si>
+  <si>
+    <t>Contrato - Autentificación MVZ</t>
+  </si>
+  <si>
+    <t>Contrato - Autentificación propietario</t>
+  </si>
+  <si>
+    <t>Contrato - Reporte administrativo</t>
+  </si>
+  <si>
+    <t>Codificación - Registrar historial médico</t>
+  </si>
+  <si>
+    <t>Codificación - Consultar historial médico</t>
+  </si>
+  <si>
+    <t>Codificación - Modificar historial médico</t>
+  </si>
+  <si>
+    <t>Codificación - Autentificación de MVZ</t>
+  </si>
+  <si>
+    <t>Codificación - Autentificación de propietario</t>
+  </si>
+  <si>
+    <t>Codificación - Reporte administrativo</t>
+  </si>
+  <si>
+    <t>Junit - Registrar historial médico</t>
+  </si>
+  <si>
+    <t>Junit - Consutar historial médico</t>
+  </si>
+  <si>
+    <t>Junit - Modificar historial médico</t>
+  </si>
+  <si>
+    <t>Junit - Autentificación de MVZ</t>
+  </si>
+  <si>
+    <t>Junit - Autentificación de propietario</t>
+  </si>
+  <si>
+    <t>Junit - Reporte administrativo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -266,11 +284,6 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -331,12 +344,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF1F497D"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -347,8 +354,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -395,8 +408,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="273">
+  <cellStyleXfs count="305">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -670,8 +707,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -686,37 +755,52 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="273">
+  <cellStyles count="305">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -853,6 +937,22 @@
     <cellStyle name="Hipervínculo" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="303" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -989,6 +1089,22 @@
     <cellStyle name="Hipervínculo visitado" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="304" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1318,15 +1434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:C34"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
@@ -1340,33 +1456,33 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="5">
@@ -1377,14 +1493,14 @@
         <v>2</v>
       </c>
       <c r="E3" s="5">
-        <f>C3*100/$D$44</f>
-        <v>1.6260162601626016</v>
+        <f>C3*100/$D$61</f>
+        <v>1.834862385321101</v>
       </c>
       <c r="F3" s="5">
         <f>E3</f>
-        <v>1.6260162601626016</v>
-      </c>
-      <c r="G3" s="18">
+        <v>1.834862385321101</v>
+      </c>
+      <c r="G3" s="15">
         <v>1</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -1393,15 +1509,15 @@
       <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>55</v>
+      <c r="K3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="5">
@@ -1412,49 +1528,49 @@
         <v>6</v>
       </c>
       <c r="E4" s="5">
-        <f>C4*100/$D$44</f>
-        <v>3.2520325203252032</v>
+        <f t="shared" ref="E4:E61" si="0">C4*100/$D$61</f>
+        <v>3.669724770642202</v>
       </c>
       <c r="F4" s="5">
         <f>E4+F3</f>
-        <v>4.8780487804878048</v>
-      </c>
-      <c r="G4" s="18"/>
+        <v>5.5045871559633035</v>
+      </c>
+      <c r="G4" s="15"/>
       <c r="H4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="10">
-        <f>SUMIF(H3:H44,"LISTO",E3:E44)</f>
-        <v>42.276422764227625</v>
-      </c>
-      <c r="L4" s="11">
+      <c r="K4" s="9">
+        <f>SUMIF(H3:H61,"LISTO",E3:E61)</f>
+        <v>70.642201834862419</v>
+      </c>
+      <c r="L4" s="10">
         <f>100-K4</f>
-        <v>57.723577235772375</v>
+        <v>29.357798165137581</v>
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="5">
         <v>4</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" ref="D5:D44" si="0">D4+C5</f>
+        <f t="shared" ref="D5:D22" si="1">D4+C5</f>
         <v>10</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E44" si="1">C5*100/$D$44</f>
-        <v>3.2520325203252032</v>
+        <f t="shared" si="0"/>
+        <v>3.669724770642202</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F44" si="2">E5+F4</f>
-        <v>8.1300813008130071</v>
-      </c>
-      <c r="G5" s="18"/>
+        <f t="shared" ref="F5:F22" si="2">E5+F4</f>
+        <v>9.1743119266055047</v>
+      </c>
+      <c r="G5" s="15"/>
       <c r="H5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1463,25 +1579,25 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
       </c>
       <c r="D6" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>8.9430894308943074</v>
-      </c>
-      <c r="G6" s="18"/>
+        <v>10.091743119266056</v>
+      </c>
+      <c r="G6" s="15"/>
       <c r="H6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1490,25 +1606,25 @@
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
       </c>
       <c r="D7" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>9.7560975609756078</v>
-      </c>
-      <c r="G7" s="18"/>
+        <v>11.009174311926607</v>
+      </c>
+      <c r="G7" s="15"/>
       <c r="H7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1517,25 +1633,25 @@
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
       </c>
       <c r="D8" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>10.569105691056908</v>
-      </c>
-      <c r="G8" s="18"/>
+        <v>11.926605504587158</v>
+      </c>
+      <c r="G8" s="15"/>
       <c r="H8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1544,52 +1660,52 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
       </c>
       <c r="D9" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>11.382113821138208</v>
-      </c>
-      <c r="G9" s="18"/>
+        <v>12.844036697247709</v>
+      </c>
+      <c r="G9" s="15"/>
       <c r="H9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
       </c>
       <c r="D10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>12.195121951219509</v>
-      </c>
-      <c r="G10" s="18"/>
+        <v>13.761467889908261</v>
+      </c>
+      <c r="G10" s="15"/>
       <c r="H10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1598,25 +1714,25 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="B11" s="8" t="s">
-        <v>39</v>
+      <c r="B11" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="5">
         <v>2</v>
       </c>
       <c r="D11" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="1"/>
-        <v>1.6260162601626016</v>
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>13.82113821138211</v>
-      </c>
-      <c r="G11" s="18">
+        <v>15.596330275229361</v>
+      </c>
+      <c r="G11" s="15">
         <v>2</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -1627,25 +1743,25 @@
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="B12" s="8" t="s">
-        <v>41</v>
+      <c r="B12" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="5">
         <v>3</v>
       </c>
       <c r="D12" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="1"/>
-        <v>2.4390243902439024</v>
+        <f t="shared" si="0"/>
+        <v>2.7522935779816513</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>16.260162601626011</v>
-      </c>
-      <c r="G12" s="18"/>
+        <v>18.348623853211013</v>
+      </c>
+      <c r="G12" s="15"/>
       <c r="H12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1654,25 +1770,25 @@
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="B13" s="8" t="s">
-        <v>42</v>
+      <c r="B13" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
       </c>
       <c r="D13" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>17.073170731707311</v>
-      </c>
-      <c r="G13" s="18"/>
+        <v>19.266055045871564</v>
+      </c>
+      <c r="G13" s="15"/>
       <c r="H13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1681,25 +1797,25 @@
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="B14" s="8" t="s">
-        <v>35</v>
+      <c r="B14" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
       </c>
       <c r="D14" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>17.886178861788611</v>
-      </c>
-      <c r="G14" s="18"/>
+        <v>20.183486238532115</v>
+      </c>
+      <c r="G14" s="15"/>
       <c r="H14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1708,25 +1824,25 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="B15" s="8" t="s">
-        <v>36</v>
+      <c r="B15" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C15" s="5">
         <v>8</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="1"/>
-        <v>6.5040650406504064</v>
+        <f t="shared" si="0"/>
+        <v>7.3394495412844041</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>24.390243902439018</v>
-      </c>
-      <c r="G15" s="18"/>
+        <v>27.522935779816521</v>
+      </c>
+      <c r="G15" s="15"/>
       <c r="H15" s="5" t="s">
         <v>11</v>
       </c>
@@ -1736,54 +1852,54 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="2"/>
-      <c r="B16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="13">
+      <c r="B16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="5">
         <v>3</v>
       </c>
-      <c r="D16" s="13">
-        <f t="shared" si="0"/>
+      <c r="D16" s="5">
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7522935779816513</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="2"/>
+        <v>30.275229357798171</v>
+      </c>
+      <c r="G16" s="15">
+        <v>3</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
         <f t="shared" si="1"/>
-        <v>2.4390243902439024</v>
-      </c>
-      <c r="F16" s="13">
-        <f t="shared" si="2"/>
-        <v>26.829268292682919</v>
-      </c>
-      <c r="G16" s="18">
-        <v>3</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5">
-        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="2"/>
-        <v>27.642276422764219</v>
-      </c>
-      <c r="G17" s="18"/>
+        <v>31.192660550458722</v>
+      </c>
+      <c r="G17" s="15"/>
       <c r="H17" s="5" t="s">
         <v>11</v>
       </c>
@@ -1792,25 +1908,25 @@
       </c>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="2"/>
-        <v>28.455284552845519</v>
-      </c>
-      <c r="G18" s="18"/>
+        <v>32.11009174311927</v>
+      </c>
+      <c r="G18" s="15"/>
       <c r="H18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1819,25 +1935,25 @@
       </c>
     </row>
     <row r="19" spans="2:9">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="2"/>
-        <v>29.26829268292682</v>
-      </c>
-      <c r="G19" s="18"/>
+        <v>33.027522935779821</v>
+      </c>
+      <c r="G19" s="15"/>
       <c r="H19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1846,25 +1962,25 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="2"/>
-        <v>30.08130081300812</v>
-      </c>
-      <c r="G20" s="18"/>
+        <v>33.944954128440372</v>
+      </c>
+      <c r="G20" s="15"/>
       <c r="H20" s="5" t="s">
         <v>11</v>
       </c>
@@ -1873,25 +1989,25 @@
       </c>
     </row>
     <row r="21" spans="2:9">
-      <c r="B21" s="8" t="s">
-        <v>43</v>
+      <c r="B21" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="2"/>
-        <v>30.89430894308942</v>
-      </c>
-      <c r="G21" s="18"/>
+        <v>34.862385321100923</v>
+      </c>
+      <c r="G21" s="15"/>
       <c r="H21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1900,25 +2016,25 @@
       </c>
     </row>
     <row r="22" spans="2:9">
-      <c r="B22" s="8" t="s">
-        <v>41</v>
+      <c r="B22" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="C22" s="5">
         <v>4</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="1"/>
-        <v>3.2520325203252032</v>
+        <f t="shared" si="0"/>
+        <v>3.669724770642202</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="2"/>
-        <v>34.146341463414622</v>
-      </c>
-      <c r="G22" s="18"/>
+        <v>38.532110091743128</v>
+      </c>
+      <c r="G22" s="15"/>
       <c r="H22" s="5" t="s">
         <v>11</v>
       </c>
@@ -1927,25 +2043,25 @@
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="5">
         <v>3</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" si="0"/>
+        <f>D22+C23</f>
         <v>45</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="1"/>
-        <v>2.4390243902439024</v>
+        <f t="shared" si="0"/>
+        <v>2.7522935779816513</v>
       </c>
       <c r="F23" s="5">
-        <f t="shared" si="2"/>
-        <v>36.585365853658523</v>
-      </c>
-      <c r="G23" s="18"/>
+        <f>E23+F22</f>
+        <v>41.284403669724782</v>
+      </c>
+      <c r="G23" s="15"/>
       <c r="H23" s="5" t="s">
         <v>11</v>
       </c>
@@ -1954,299 +2070,299 @@
       </c>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="4">
-        <v>3</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="0"/>
+      <c r="B24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" ref="D24:D61" si="3">D23+C24</f>
+        <v>46</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" ref="F24:F61" si="4">E24+F23</f>
+        <v>42.201834862385333</v>
+      </c>
+      <c r="G24" s="16">
+        <v>4</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="5">
-        <f t="shared" si="1"/>
-        <v>2.4390243902439024</v>
-      </c>
-      <c r="F24" s="4">
-        <f t="shared" si="2"/>
-        <v>39.024390243902424</v>
-      </c>
-      <c r="G24" s="17">
-        <v>4</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9">
-      <c r="B25" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="4">
-        <v>8</v>
-      </c>
-      <c r="D25" s="4">
-        <f t="shared" si="0"/>
-        <v>56</v>
+      <c r="C25" s="14">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="3"/>
+        <v>47</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="1"/>
-        <v>6.5040650406504064</v>
-      </c>
-      <c r="F25" s="4">
-        <f t="shared" si="2"/>
-        <v>45.528455284552834</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="4"/>
+        <v>43.119266055045884</v>
       </c>
       <c r="G25" s="17"/>
-      <c r="H25" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>19</v>
+      <c r="H25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:9">
-      <c r="B26" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="4">
-        <v>3</v>
-      </c>
-      <c r="D26" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
+      <c r="B26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="14">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="3"/>
+        <v>48</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="1"/>
-        <v>2.4390243902439024</v>
-      </c>
-      <c r="F26" s="4">
-        <f t="shared" si="2"/>
-        <v>47.967479674796735</v>
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="4"/>
+        <v>44.036697247706435</v>
       </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>21</v>
+      <c r="H26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:9">
-      <c r="B27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="5">
+      <c r="B27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="14">
         <v>2</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="0"/>
-        <v>61</v>
+        <f t="shared" si="3"/>
+        <v>50</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" si="1"/>
-        <v>1.6260162601626016</v>
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
       </c>
       <c r="F27" s="5">
-        <f t="shared" si="2"/>
-        <v>49.593495934959336</v>
+        <f t="shared" si="4"/>
+        <v>45.871559633027537</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>57</v>
+      <c r="I27" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:9">
-      <c r="B28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="5">
+      <c r="B28" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="14">
+        <v>3</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7522935779816513</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="4"/>
+        <v>48.623853211009191</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="14">
         <v>2</v>
       </c>
-      <c r="D28" s="5">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="E28" s="5">
-        <f t="shared" si="1"/>
-        <v>1.6260162601626016</v>
-      </c>
-      <c r="F28" s="5">
-        <f t="shared" si="2"/>
-        <v>51.219512195121936</v>
-      </c>
-      <c r="G28" s="17">
-        <v>5</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9">
-      <c r="B29" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="5">
-        <v>2</v>
-      </c>
       <c r="D29" s="5">
-        <f t="shared" si="0"/>
-        <v>65</v>
+        <f t="shared" si="3"/>
+        <v>55</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="1"/>
-        <v>1.6260162601626016</v>
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
       </c>
       <c r="F29" s="5">
-        <f t="shared" si="2"/>
-        <v>52.845528455284537</v>
+        <f t="shared" si="4"/>
+        <v>50.458715596330293</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I29" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="14">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="4"/>
+        <v>51.376146788990845</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="14">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="2:9">
-      <c r="B30" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="4">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="E30" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
-      </c>
-      <c r="F30" s="4">
-        <f t="shared" si="2"/>
-        <v>53.658536585365837</v>
-      </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I30" s="4" t="s">
+      <c r="E31" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="4"/>
+        <v>52.293577981651396</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="14">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F32" s="5">
+        <f t="shared" si="4"/>
+        <v>53.211009174311947</v>
+      </c>
+      <c r="G32" s="17"/>
+      <c r="H32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:9">
-      <c r="B31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="4">
+    <row r="33" spans="2:9">
+      <c r="B33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="14">
+        <v>3</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7522935779816513</v>
+      </c>
+      <c r="F33" s="5">
+        <f t="shared" si="4"/>
+        <v>55.9633027522936</v>
+      </c>
+      <c r="G33" s="18"/>
+      <c r="H33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="5">
         <v>2</v>
       </c>
-      <c r="D31" s="4">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="E31" s="5">
-        <f t="shared" si="1"/>
-        <v>1.6260162601626016</v>
-      </c>
-      <c r="F31" s="4">
-        <f t="shared" si="2"/>
-        <v>55.284552845528438</v>
-      </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9">
-      <c r="B32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="4">
-        <v>2</v>
-      </c>
-      <c r="D32" s="4">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="E32" s="5">
-        <f t="shared" si="1"/>
-        <v>1.6260162601626016</v>
-      </c>
-      <c r="F32" s="4">
-        <f t="shared" si="2"/>
-        <v>56.910569105691039</v>
-      </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9">
-      <c r="B33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="4">
-        <v>2</v>
-      </c>
-      <c r="D33" s="4">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="E33" s="5">
-        <f t="shared" si="1"/>
-        <v>1.6260162601626016</v>
-      </c>
-      <c r="F33" s="4">
-        <f t="shared" si="2"/>
-        <v>58.536585365853639</v>
-      </c>
-      <c r="G33" s="17"/>
-      <c r="H33" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9">
-      <c r="B34" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="5">
-        <v>4</v>
-      </c>
       <c r="D34" s="5">
-        <f t="shared" si="0"/>
-        <v>76</v>
+        <f t="shared" si="3"/>
+        <v>63</v>
       </c>
       <c r="E34" s="5">
-        <f t="shared" si="1"/>
-        <v>3.2520325203252032</v>
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
       </c>
       <c r="F34" s="5">
-        <f t="shared" si="2"/>
-        <v>61.788617886178841</v>
-      </c>
-      <c r="G34" s="17"/>
+        <f t="shared" si="4"/>
+        <v>57.798165137614703</v>
+      </c>
+      <c r="G34" s="16">
+        <v>5</v>
+      </c>
       <c r="H34" s="5" t="s">
         <v>11</v>
       </c>
@@ -2255,311 +2371,833 @@
       </c>
     </row>
     <row r="35" spans="2:9">
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="5">
+        <v>2</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F35" s="5">
+        <f t="shared" si="4"/>
+        <v>59.633027522935805</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="H35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="5">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F36" s="5">
+        <f t="shared" si="4"/>
+        <v>61.467889908256907</v>
+      </c>
+      <c r="G36" s="17"/>
+      <c r="H36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="4"/>
+        <v>63.30275229357801</v>
+      </c>
+      <c r="G37" s="17"/>
+      <c r="H37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="5">
+        <v>2</v>
+      </c>
+      <c r="D38" s="5">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="4"/>
+        <v>65.137614678899112</v>
+      </c>
+      <c r="G38" s="17"/>
+      <c r="H38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="5">
+        <v>2</v>
+      </c>
+      <c r="D39" s="5">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="4"/>
+        <v>66.972477064220215</v>
+      </c>
+      <c r="G39" s="17"/>
+      <c r="H39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="5">
+        <v>2</v>
+      </c>
+      <c r="D40" s="5">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" si="4"/>
+        <v>68.807339449541317</v>
+      </c>
+      <c r="G40" s="17"/>
+      <c r="H40" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="5">
+        <v>2</v>
+      </c>
+      <c r="D41" s="5">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="E41" s="5">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F41" s="5">
+        <f t="shared" si="4"/>
+        <v>70.642201834862419</v>
+      </c>
+      <c r="G41" s="18"/>
+      <c r="H41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="19">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="E42" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F42" s="4">
+        <f t="shared" si="4"/>
+        <v>71.559633027522963</v>
+      </c>
+      <c r="G42" s="20">
+        <v>6</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="19">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="E43" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F43" s="4">
+        <f t="shared" si="4"/>
+        <v>72.477064220183507</v>
+      </c>
+      <c r="G43" s="21"/>
+      <c r="H43" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="E44" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F44" s="4">
+        <f t="shared" si="4"/>
+        <v>73.394495412844051</v>
+      </c>
+      <c r="G44" s="21"/>
+      <c r="H44" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F45" s="4">
+        <f t="shared" si="4"/>
+        <v>74.311926605504595</v>
+      </c>
+      <c r="G45" s="21"/>
+      <c r="H45" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="E46" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F46" s="4">
+        <f t="shared" si="4"/>
+        <v>75.22935779816514</v>
+      </c>
+      <c r="G46" s="21"/>
+      <c r="H46" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9">
+      <c r="B47" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+      <c r="E47" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F47" s="4">
+        <f t="shared" si="4"/>
+        <v>76.146788990825684</v>
+      </c>
+      <c r="G47" s="21"/>
+      <c r="H47" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9">
+      <c r="B48" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="4">
+        <v>2</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="3"/>
+        <v>85</v>
+      </c>
+      <c r="E48" s="4">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F48" s="4">
+        <f t="shared" si="4"/>
+        <v>77.981651376146786</v>
+      </c>
+      <c r="G48" s="21"/>
+      <c r="H48" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9">
+      <c r="B49" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="4">
+        <v>2</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+      <c r="E49" s="4">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F49" s="4">
+        <f t="shared" si="4"/>
+        <v>79.816513761467888</v>
+      </c>
+      <c r="G49" s="21"/>
+      <c r="H49" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I49" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9">
+      <c r="B50" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="4">
+        <v>2</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="E50" s="4">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F50" s="4">
+        <f t="shared" si="4"/>
+        <v>81.651376146788991</v>
+      </c>
+      <c r="G50" s="21"/>
+      <c r="H50" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9">
+      <c r="B51" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="4">
+        <v>2</v>
+      </c>
+      <c r="D51" s="4">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+      <c r="E51" s="4">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F51" s="4">
+        <f t="shared" si="4"/>
+        <v>83.486238532110093</v>
+      </c>
+      <c r="G51" s="21"/>
+      <c r="H51" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9">
+      <c r="B52" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="4">
+        <v>2</v>
+      </c>
+      <c r="D52" s="4">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="E52" s="4">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F52" s="4">
+        <f t="shared" si="4"/>
+        <v>85.321100917431195</v>
+      </c>
+      <c r="G52" s="21"/>
+      <c r="H52" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9">
+      <c r="B53" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="4">
+        <v>2</v>
+      </c>
+      <c r="D53" s="4">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+      <c r="E53" s="4">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F53" s="4">
+        <f t="shared" si="4"/>
+        <v>87.155963302752298</v>
+      </c>
+      <c r="G53" s="20">
+        <v>7</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="B54" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="4">
+        <v>1</v>
+      </c>
+      <c r="D54" s="4">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+      <c r="E54" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F54" s="4">
+        <f t="shared" si="4"/>
+        <v>88.073394495412842</v>
+      </c>
+      <c r="G54" s="21"/>
+      <c r="H54" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9">
+      <c r="B55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="4">
+        <v>1</v>
+      </c>
+      <c r="D55" s="4">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="E55" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F55" s="4">
+        <f t="shared" si="4"/>
+        <v>88.990825688073386</v>
+      </c>
+      <c r="G55" s="21"/>
+      <c r="H55" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9">
+      <c r="B56" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+      <c r="D56" s="4">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="E56" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F56" s="4">
+        <f t="shared" si="4"/>
+        <v>89.90825688073393</v>
+      </c>
+      <c r="G56" s="21"/>
+      <c r="H56" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9">
+      <c r="B57" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1</v>
+      </c>
+      <c r="D57" s="4">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+      <c r="E57" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F57" s="4">
+        <f t="shared" si="4"/>
+        <v>90.825688073394474</v>
+      </c>
+      <c r="G57" s="21"/>
+      <c r="H57" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9">
+      <c r="B58" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="4">
+        <v>1</v>
+      </c>
+      <c r="D58" s="4">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="E58" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F58" s="4">
+        <f t="shared" si="4"/>
+        <v>91.743119266055018</v>
+      </c>
+      <c r="G58" s="21"/>
+      <c r="H58" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I58" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9">
+      <c r="B59" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" s="4">
+        <v>1</v>
+      </c>
+      <c r="D59" s="4">
+        <f t="shared" si="3"/>
+        <v>101</v>
+      </c>
+      <c r="E59" s="4">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F59" s="4">
+        <f t="shared" si="4"/>
+        <v>92.660550458715562</v>
+      </c>
+      <c r="G59" s="21"/>
+      <c r="H59" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9">
+      <c r="B60" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="4">
+        <v>4</v>
+      </c>
+      <c r="D60" s="4">
+        <f t="shared" si="3"/>
+        <v>105</v>
+      </c>
+      <c r="E60" s="4">
+        <f t="shared" si="0"/>
+        <v>3.669724770642202</v>
+      </c>
+      <c r="F60" s="4">
+        <f t="shared" si="4"/>
+        <v>96.330275229357767</v>
+      </c>
+      <c r="G60" s="21"/>
+      <c r="H60" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9">
+      <c r="B61" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="4">
-        <v>6</v>
-      </c>
-      <c r="D35" s="4">
-        <f t="shared" si="0"/>
-        <v>82</v>
-      </c>
-      <c r="E35" s="5">
-        <f t="shared" si="1"/>
-        <v>4.8780487804878048</v>
-      </c>
-      <c r="F35" s="4">
-        <f t="shared" si="2"/>
-        <v>66.666666666666643</v>
-      </c>
-      <c r="G35" s="17">
-        <v>6</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I35" s="6" t="s">
+      <c r="C61" s="4">
+        <v>4</v>
+      </c>
+      <c r="D61" s="4">
+        <f t="shared" si="3"/>
+        <v>109</v>
+      </c>
+      <c r="E61" s="4">
+        <f t="shared" si="0"/>
+        <v>3.669724770642202</v>
+      </c>
+      <c r="F61" s="4">
+        <f t="shared" si="4"/>
+        <v>99.999999999999972</v>
+      </c>
+      <c r="G61" s="23"/>
+      <c r="H61" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
-      <c r="B36" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="4">
-        <v>1</v>
-      </c>
-      <c r="D36" s="4">
-        <f t="shared" si="0"/>
-        <v>83</v>
-      </c>
-      <c r="E36" s="5">
-        <f t="shared" si="1"/>
-        <v>0.81300813008130079</v>
-      </c>
-      <c r="F36" s="4">
-        <f t="shared" si="2"/>
-        <v>67.479674796747943</v>
-      </c>
-      <c r="G36" s="17"/>
-      <c r="H36" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9">
-      <c r="B37" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="4">
-        <v>2</v>
-      </c>
-      <c r="D37" s="4">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="E37" s="5">
-        <f t="shared" si="1"/>
-        <v>1.6260162601626016</v>
-      </c>
-      <c r="F37" s="4">
-        <f t="shared" si="2"/>
-        <v>69.105691056910544</v>
-      </c>
-      <c r="G37" s="17"/>
-      <c r="H37" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9">
-      <c r="B38" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="4">
-        <v>3</v>
-      </c>
-      <c r="D38" s="4">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="E38" s="5">
-        <f t="shared" si="1"/>
-        <v>2.4390243902439024</v>
-      </c>
-      <c r="F38" s="4">
-        <f t="shared" si="2"/>
-        <v>71.544715447154445</v>
-      </c>
-      <c r="G38" s="17"/>
-      <c r="H38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9">
-      <c r="B39" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="4">
-        <v>3</v>
-      </c>
-      <c r="D39" s="4">
-        <f t="shared" si="0"/>
-        <v>91</v>
-      </c>
-      <c r="E39" s="5">
-        <f t="shared" si="1"/>
-        <v>2.4390243902439024</v>
-      </c>
-      <c r="F39" s="4">
-        <f t="shared" si="2"/>
-        <v>73.983739837398346</v>
-      </c>
-      <c r="G39" s="17"/>
-      <c r="H39" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9">
-      <c r="B40" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="4">
-        <v>10</v>
-      </c>
-      <c r="D40" s="4">
-        <f t="shared" si="0"/>
-        <v>101</v>
-      </c>
-      <c r="E40" s="5">
-        <f t="shared" si="1"/>
-        <v>8.1300813008130088</v>
-      </c>
-      <c r="F40" s="4">
-        <f t="shared" si="2"/>
-        <v>82.11382113821135</v>
-      </c>
-      <c r="G40" s="17">
-        <v>7</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9">
-      <c r="B41" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="4">
-        <v>6</v>
-      </c>
-      <c r="D41" s="4">
-        <f t="shared" si="0"/>
-        <v>107</v>
-      </c>
-      <c r="E41" s="5">
-        <f t="shared" si="1"/>
-        <v>4.8780487804878048</v>
-      </c>
-      <c r="F41" s="4">
-        <f t="shared" si="2"/>
-        <v>86.991869918699152</v>
-      </c>
-      <c r="G41" s="17"/>
-      <c r="H41" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9">
-      <c r="B42" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="4">
-        <v>4</v>
-      </c>
-      <c r="D42" s="4">
-        <f t="shared" si="0"/>
-        <v>111</v>
-      </c>
-      <c r="E42" s="5">
-        <f t="shared" si="1"/>
-        <v>3.2520325203252032</v>
-      </c>
-      <c r="F42" s="4">
-        <f t="shared" si="2"/>
-        <v>90.243902439024353</v>
-      </c>
-      <c r="G42" s="17">
-        <v>8</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9">
-      <c r="B43" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="4">
-        <v>6</v>
-      </c>
-      <c r="D43" s="4">
-        <f t="shared" si="0"/>
-        <v>117</v>
-      </c>
-      <c r="E43" s="5">
-        <f t="shared" si="1"/>
-        <v>4.8780487804878048</v>
-      </c>
-      <c r="F43" s="4">
-        <f t="shared" si="2"/>
-        <v>95.121951219512155</v>
-      </c>
-      <c r="G43" s="17"/>
-      <c r="H43" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9">
-      <c r="B44" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="4">
-        <v>6</v>
-      </c>
-      <c r="D44" s="4">
-        <f t="shared" si="0"/>
-        <v>123</v>
-      </c>
-      <c r="E44" s="5">
-        <f t="shared" si="1"/>
-        <v>4.8780487804878048</v>
-      </c>
-      <c r="F44" s="4">
-        <f t="shared" si="2"/>
-        <v>99.999999999999957</v>
-      </c>
-      <c r="G44" s="17"/>
-      <c r="H44" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9">
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="2:9">
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="2:9">
-      <c r="H47" s="1"/>
-      <c r="I47"/>
+    <row r="62" spans="2:9">
+      <c r="I62"/>
+    </row>
+    <row r="63" spans="2:9">
+      <c r="I63"/>
+    </row>
+    <row r="64" spans="2:9">
+      <c r="I64"/>
+    </row>
+    <row r="65" spans="9:9">
+      <c r="I65"/>
+    </row>
+    <row r="66" spans="9:9">
+      <c r="I66"/>
+    </row>
+    <row r="67" spans="9:9">
+      <c r="I67"/>
+    </row>
+    <row r="68" spans="9:9">
+      <c r="I68"/>
+    </row>
+    <row r="69" spans="9:9">
+      <c r="I69"/>
+    </row>
+    <row r="70" spans="9:9">
+      <c r="I70"/>
+    </row>
+    <row r="71" spans="9:9">
+      <c r="I71"/>
+    </row>
+    <row r="72" spans="9:9">
+      <c r="I72"/>
+    </row>
+    <row r="73" spans="9:9">
+      <c r="I73"/>
+    </row>
+    <row r="74" spans="9:9">
+      <c r="I74"/>
+    </row>
+    <row r="75" spans="9:9">
+      <c r="I75"/>
+    </row>
+    <row r="76" spans="9:9">
+      <c r="I76"/>
+    </row>
+    <row r="77" spans="9:9">
+      <c r="I77"/>
+    </row>
+    <row r="78" spans="9:9">
+      <c r="I78"/>
+    </row>
+    <row r="79" spans="9:9">
+      <c r="I79"/>
+    </row>
+    <row r="80" spans="9:9">
+      <c r="I80"/>
+    </row>
+    <row r="81" spans="3:9">
+      <c r="I81"/>
+    </row>
+    <row r="82" spans="3:9">
+      <c r="I82"/>
+    </row>
+    <row r="83" spans="3:9">
+      <c r="I83"/>
+    </row>
+    <row r="84" spans="3:9">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="2"/>
+    </row>
+    <row r="85" spans="3:9">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="3:9">
+      <c r="H86" s="1"/>
+      <c r="I86"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="G35:G39"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="G42:G44"/>
+  <mergeCells count="7">
     <mergeCell ref="G3:G10"/>
     <mergeCell ref="G11:G15"/>
     <mergeCell ref="G16:G23"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="G28:G34"/>
+    <mergeCell ref="G24:G33"/>
+    <mergeCell ref="G34:G41"/>
+    <mergeCell ref="G42:G52"/>
+    <mergeCell ref="G53:G61"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2576,7 +3214,7 @@
   <dimension ref="B4:D14"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2586,123 +3224,123 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="16">
-        <v>1</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="B5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="16">
-        <v>1</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>69</v>
+      <c r="B6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="16">
-        <v>1</v>
-      </c>
-      <c r="D7" s="16" t="s">
+      <c r="B7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="16">
+      <c r="B8" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="14">
         <v>2</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="16">
+      <c r="B9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="14">
         <v>3</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>69</v>
+      <c r="D9" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="16">
+      <c r="B10" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="14">
         <v>2</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="16">
-        <v>1</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="B11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="16">
-        <v>1</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>69</v>
+      <c r="B12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="2:4">
-      <c r="B13" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="16">
-        <v>1</v>
-      </c>
-      <c r="D13" s="16" t="s">
+      <c r="B13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:4">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="14">
         <v>3</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2721,8 +3359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2733,18 +3371,18 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:4">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="5">
@@ -2755,7 +3393,7 @@
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="5">
@@ -2766,18 +3404,18 @@
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="8" t="s">
-        <v>38</v>
+      <c r="B7" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="5">
@@ -2788,7 +3426,7 @@
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="5">
@@ -2799,19 +3437,19 @@
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="8" t="s">
-        <v>70</v>
+      <c r="B11" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="C11" s="5">
         <v>2</v>
@@ -2821,8 +3459,8 @@
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="8" t="s">
-        <v>71</v>
+      <c r="B12" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="C12" s="5">
         <v>2</v>
@@ -2833,6 +3471,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Se modifica .gitignore para no hacer seguimiento a las configuraciones locales de netbeans, se modifica el diagrama de casos de uso (se agrega DAOpropietario), se modifica calendario, se modifica la clase conexion para que los atributos queden privados y no publicos
</commit_message>
<xml_diff>
--- a/documentos/General/CronogramaTSP.xlsx
+++ b/documentos/General/CronogramaTSP.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Cronograma General" sheetId="1" r:id="rId1"/>
     <sheet name="Cuarta Semana" sheetId="3" r:id="rId2"/>
     <sheet name="Quinta Semana" sheetId="4" r:id="rId3"/>
+    <sheet name="Sexta Semana" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="81">
   <si>
     <t>Tarea</t>
   </si>
@@ -41,9 +42,6 @@
     <t>Semana</t>
   </si>
   <si>
-    <t>VG</t>
-  </si>
-  <si>
     <t>Entrevista con MVZ</t>
   </si>
   <si>
@@ -255,6 +253,18 @@
   </si>
   <si>
     <t>Junit - Reporte administrativo</t>
+  </si>
+  <si>
+    <t>Juan Esteban</t>
+  </si>
+  <si>
+    <t>Valor Ganado</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>TRI</t>
   </si>
 </sst>
 </file>
@@ -317,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +367,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -433,7 +449,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="305">
+  <cellStyleXfs count="323">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -739,8 +755,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -772,6 +806,24 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -784,23 +836,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="305">
+  <cellStyles count="323">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -953,6 +1011,15 @@
     <cellStyle name="Hipervínculo" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="301" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="321" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -1105,6 +1172,15 @@
     <cellStyle name="Hipervínculo visitado" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="302" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="322" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1434,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:N86"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1447,15 +1523,17 @@
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" customWidth="1"/>
+    <col min="11" max="11" width="18" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1475,15 +1553,21 @@
         <v>5</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="B3" s="7" t="s">
-        <v>7</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
@@ -1500,25 +1584,27 @@
         <f>E3</f>
         <v>1.834862385321101</v>
       </c>
-      <c r="G3" s="15">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="11" t="s">
+      <c r="G3" s="28">
+        <v>1</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+    </row>
+    <row r="4" spans="1:14">
       <c r="B4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5">
         <v>4</v>
@@ -1535,25 +1621,27 @@
         <f>E4+F3</f>
         <v>5.5045871559633035</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="9">
-        <f>SUMIF(H3:H61,"LISTO",E3:E61)</f>
+      <c r="G4" s="28"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="9">
+        <f>SUMIF(J3:J61,"LISTO",E3:E61)</f>
         <v>70.642201834862419</v>
       </c>
-      <c r="L4" s="10">
-        <f>100-K4</f>
+      <c r="N4" s="10">
+        <f>100-M4</f>
         <v>29.357798165137581</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="B5" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5">
         <v>4</v>
@@ -1570,17 +1658,19 @@
         <f t="shared" ref="F5:F22" si="2">E5+F4</f>
         <v>9.1743119266055047</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="G5" s="28"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="B6" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -1597,17 +1687,19 @@
         <f t="shared" si="2"/>
         <v>10.091743119266056</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="G6" s="28"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -1624,17 +1716,19 @@
         <f t="shared" si="2"/>
         <v>11.009174311926607</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="G7" s="28"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="B8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -1651,17 +1745,19 @@
         <f t="shared" si="2"/>
         <v>11.926605504587158</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="G8" s="28"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1678,17 +1774,19 @@
         <f t="shared" si="2"/>
         <v>12.844036697247709</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="G9" s="28"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1705,17 +1803,19 @@
         <f t="shared" si="2"/>
         <v>13.761467889908261</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="G10" s="28"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="B11" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="5">
         <v>2</v>
@@ -1732,19 +1832,21 @@
         <f t="shared" si="2"/>
         <v>15.596330275229361</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="28">
         <v>2</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="B12" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="5">
         <v>3</v>
@@ -1761,17 +1863,19 @@
         <f t="shared" si="2"/>
         <v>18.348623853211013</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="G12" s="28"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="B13" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1788,17 +1892,19 @@
         <f t="shared" si="2"/>
         <v>19.266055045871564</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="G13" s="28"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="B14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -1815,17 +1921,19 @@
         <f t="shared" si="2"/>
         <v>20.183486238532115</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="G14" s="28"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="B15" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="5">
         <v>8</v>
@@ -1842,18 +1950,20 @@
         <f t="shared" si="2"/>
         <v>27.522935779816521</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="G15" s="28"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="2"/>
       <c r="B16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="5">
         <v>3</v>
@@ -1870,19 +1980,21 @@
         <f t="shared" si="2"/>
         <v>30.275229357798171</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="28">
         <v>3</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9">
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
       <c r="B17" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -1899,17 +2011,19 @@
         <f t="shared" si="2"/>
         <v>31.192660550458722</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9">
+      <c r="G17" s="28"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
       <c r="B18" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -1926,17 +2040,19 @@
         <f t="shared" si="2"/>
         <v>32.11009174311927</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="5" t="s">
+      <c r="G18" s="28"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -1953,17 +2069,19 @@
         <f t="shared" si="2"/>
         <v>33.027522935779821</v>
       </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9">
+      <c r="G19" s="28"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
       <c r="B20" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -1980,17 +2098,19 @@
         <f t="shared" si="2"/>
         <v>33.944954128440372</v>
       </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9">
+      <c r="G20" s="28"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
       <c r="B21" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -2007,17 +2127,19 @@
         <f t="shared" si="2"/>
         <v>34.862385321100923</v>
       </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9">
+      <c r="G21" s="28"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="5">
         <v>4</v>
@@ -2034,17 +2156,19 @@
         <f t="shared" si="2"/>
         <v>38.532110091743128</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9">
+      <c r="G22" s="28"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
       <c r="B23" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="5">
         <v>3</v>
@@ -2061,17 +2185,19 @@
         <f>E23+F22</f>
         <v>41.284403669724782</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9">
+      <c r="G23" s="28"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
       <c r="B24" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="14">
         <v>1</v>
@@ -2088,19 +2214,21 @@
         <f t="shared" ref="F24:F61" si="4">E24+F23</f>
         <v>42.201834862385333</v>
       </c>
-      <c r="G24" s="16">
+      <c r="G24" s="29">
         <v>4</v>
       </c>
-      <c r="H24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9">
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
       <c r="B25" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="14">
         <v>1</v>
@@ -2117,17 +2245,19 @@
         <f t="shared" si="4"/>
         <v>43.119266055045884</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9">
+      <c r="G25" s="30"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
       <c r="B26" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="14">
         <v>1</v>
@@ -2144,17 +2274,19 @@
         <f t="shared" si="4"/>
         <v>44.036697247706435</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9">
+      <c r="G26" s="30"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
       <c r="B27" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" s="14">
         <v>2</v>
@@ -2171,17 +2303,19 @@
         <f t="shared" si="4"/>
         <v>45.871559633027537</v>
       </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9">
+      <c r="G27" s="30"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
       <c r="B28" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="14">
         <v>3</v>
@@ -2198,17 +2332,19 @@
         <f t="shared" si="4"/>
         <v>48.623853211009191</v>
       </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9">
+      <c r="G28" s="30"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11">
       <c r="B29" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="14">
         <v>2</v>
@@ -2225,17 +2361,19 @@
         <f t="shared" si="4"/>
         <v>50.458715596330293</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9">
+      <c r="G29" s="30"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
       <c r="B30" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="14">
         <v>1</v>
@@ -2252,17 +2390,19 @@
         <f t="shared" si="4"/>
         <v>51.376146788990845</v>
       </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9">
+      <c r="G30" s="30"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11">
       <c r="B31" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="14">
         <v>1</v>
@@ -2279,17 +2419,19 @@
         <f t="shared" si="4"/>
         <v>52.293577981651396</v>
       </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9">
+      <c r="G31" s="30"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11">
       <c r="B32" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="14">
         <v>1</v>
@@ -2306,17 +2448,19 @@
         <f t="shared" si="4"/>
         <v>53.211009174311947</v>
       </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I32" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9">
+      <c r="G32" s="30"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
       <c r="B33" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="14">
         <v>3</v>
@@ -2333,17 +2477,19 @@
         <f t="shared" si="4"/>
         <v>55.9633027522936</v>
       </c>
-      <c r="G33" s="18"/>
-      <c r="H33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9">
+      <c r="G33" s="31"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11">
       <c r="B34" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="5">
         <v>2</v>
@@ -2360,19 +2506,21 @@
         <f t="shared" si="4"/>
         <v>57.798165137614703</v>
       </c>
-      <c r="G34" s="16">
+      <c r="G34" s="29">
         <v>5</v>
       </c>
-      <c r="H34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9">
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11">
       <c r="B35" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" s="5">
         <v>2</v>
@@ -2389,17 +2537,19 @@
         <f t="shared" si="4"/>
         <v>59.633027522935805</v>
       </c>
-      <c r="G35" s="17"/>
-      <c r="H35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9">
+      <c r="G35" s="30"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11">
       <c r="B36" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36" s="5">
         <v>2</v>
@@ -2416,17 +2566,19 @@
         <f t="shared" si="4"/>
         <v>61.467889908256907</v>
       </c>
-      <c r="G36" s="17"/>
-      <c r="H36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9">
+      <c r="G36" s="30"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
       <c r="B37" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C37" s="5">
         <v>2</v>
@@ -2443,17 +2595,19 @@
         <f t="shared" si="4"/>
         <v>63.30275229357801</v>
       </c>
-      <c r="G37" s="17"/>
-      <c r="H37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9">
+      <c r="G37" s="30"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11">
       <c r="B38" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C38" s="5">
         <v>2</v>
@@ -2470,17 +2624,19 @@
         <f t="shared" si="4"/>
         <v>65.137614678899112</v>
       </c>
-      <c r="G38" s="17"/>
-      <c r="H38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9">
+      <c r="G38" s="30"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11">
       <c r="B39" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="5">
         <v>2</v>
@@ -2497,17 +2653,19 @@
         <f t="shared" si="4"/>
         <v>66.972477064220215</v>
       </c>
-      <c r="G39" s="17"/>
-      <c r="H39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I39" s="5" t="s">
+      <c r="G39" s="30"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="7" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9">
-      <c r="B40" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="C40" s="5">
         <v>2</v>
@@ -2524,17 +2682,19 @@
         <f t="shared" si="4"/>
         <v>68.807339449541317</v>
       </c>
-      <c r="G40" s="17"/>
-      <c r="H40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9">
+      <c r="G40" s="30"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11">
       <c r="B41" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="5">
         <v>2</v>
@@ -2551,19 +2711,21 @@
         <f t="shared" si="4"/>
         <v>70.642201834862419</v>
       </c>
-      <c r="G41" s="18"/>
-      <c r="H41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9">
+      <c r="G41" s="31"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11">
       <c r="B42" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="19">
+        <v>59</v>
+      </c>
+      <c r="C42" s="15">
         <v>1</v>
       </c>
       <c r="D42" s="4">
@@ -2578,21 +2740,23 @@
         <f t="shared" si="4"/>
         <v>71.559633027522963</v>
       </c>
-      <c r="G42" s="20">
+      <c r="G42" s="25">
         <v>6</v>
       </c>
-      <c r="H42" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I42" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9">
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11">
       <c r="B43" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="19">
+        <v>60</v>
+      </c>
+      <c r="C43" s="15">
         <v>1</v>
       </c>
       <c r="D43" s="4">
@@ -2607,17 +2771,19 @@
         <f t="shared" si="4"/>
         <v>72.477064220183507</v>
       </c>
-      <c r="G43" s="21"/>
-      <c r="H43" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9">
+      <c r="G43" s="26"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11">
       <c r="B44" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44" s="4">
         <v>1</v>
@@ -2634,17 +2800,19 @@
         <f t="shared" si="4"/>
         <v>73.394495412844051</v>
       </c>
-      <c r="G44" s="21"/>
-      <c r="H44" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9">
+      <c r="G44" s="26"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11">
       <c r="B45" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" s="4">
         <v>1</v>
@@ -2661,17 +2829,19 @@
         <f t="shared" si="4"/>
         <v>74.311926605504595</v>
       </c>
-      <c r="G45" s="21"/>
-      <c r="H45" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I45" s="4" t="s">
+      <c r="G45" s="26"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K45" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="2:11">
       <c r="B46" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" s="4">
         <v>1</v>
@@ -2688,17 +2858,19 @@
         <f t="shared" si="4"/>
         <v>75.22935779816514</v>
       </c>
-      <c r="G46" s="21"/>
-      <c r="H46" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9">
+      <c r="G46" s="26"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11">
       <c r="B47" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="4">
         <v>1</v>
@@ -2715,17 +2887,19 @@
         <f t="shared" si="4"/>
         <v>76.146788990825684</v>
       </c>
-      <c r="G47" s="21"/>
-      <c r="H47" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9">
+      <c r="G47" s="26"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11">
       <c r="B48" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="4">
         <v>2</v>
@@ -2742,17 +2916,19 @@
         <f t="shared" si="4"/>
         <v>77.981651376146786</v>
       </c>
-      <c r="G48" s="21"/>
-      <c r="H48" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9">
+      <c r="G48" s="26"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11">
       <c r="B49" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49" s="4">
         <v>2</v>
@@ -2769,17 +2945,19 @@
         <f t="shared" si="4"/>
         <v>79.816513761467888</v>
       </c>
-      <c r="G49" s="21"/>
-      <c r="H49" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I49" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9">
+      <c r="G49" s="26"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11">
       <c r="B50" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="4">
         <v>2</v>
@@ -2796,17 +2974,19 @@
         <f t="shared" si="4"/>
         <v>81.651376146788991</v>
       </c>
-      <c r="G50" s="21"/>
-      <c r="H50" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I50" s="4" t="s">
+      <c r="G50" s="26"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K50" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:11">
       <c r="B51" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51" s="4">
         <v>2</v>
@@ -2823,17 +3003,19 @@
         <f t="shared" si="4"/>
         <v>83.486238532110093</v>
       </c>
-      <c r="G51" s="21"/>
-      <c r="H51" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9">
+      <c r="G51" s="26"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11">
       <c r="B52" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="4">
         <v>2</v>
@@ -2850,17 +3032,19 @@
         <f t="shared" si="4"/>
         <v>85.321100917431195</v>
       </c>
-      <c r="G52" s="21"/>
-      <c r="H52" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9">
+      <c r="G52" s="26"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11">
       <c r="B53" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53" s="4">
         <v>2</v>
@@ -2877,19 +3061,21 @@
         <f t="shared" si="4"/>
         <v>87.155963302752298</v>
       </c>
-      <c r="G53" s="20">
+      <c r="G53" s="25">
         <v>7</v>
       </c>
-      <c r="H53" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9">
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11">
       <c r="B54" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54" s="4">
         <v>1</v>
@@ -2906,17 +3092,19 @@
         <f t="shared" si="4"/>
         <v>88.073394495412842</v>
       </c>
-      <c r="G54" s="21"/>
-      <c r="H54" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I54" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9">
+      <c r="G54" s="26"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K54" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11">
       <c r="B55" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" s="4">
         <v>1</v>
@@ -2933,17 +3121,19 @@
         <f t="shared" si="4"/>
         <v>88.990825688073386</v>
       </c>
-      <c r="G55" s="21"/>
-      <c r="H55" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9">
+      <c r="G55" s="26"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11">
       <c r="B56" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56" s="4">
         <v>1</v>
@@ -2960,17 +3150,19 @@
         <f t="shared" si="4"/>
         <v>89.90825688073393</v>
       </c>
-      <c r="G56" s="21"/>
-      <c r="H56" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I56" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9">
+      <c r="G56" s="26"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11">
       <c r="B57" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C57" s="4">
         <v>1</v>
@@ -2987,17 +3179,19 @@
         <f t="shared" si="4"/>
         <v>90.825688073394474</v>
       </c>
-      <c r="G57" s="21"/>
-      <c r="H57" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9">
+      <c r="G57" s="26"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11">
       <c r="B58" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C58" s="4">
         <v>1</v>
@@ -3014,17 +3208,19 @@
         <f t="shared" si="4"/>
         <v>91.743119266055018</v>
       </c>
-      <c r="G58" s="21"/>
-      <c r="H58" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I58" s="22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9">
+      <c r="G58" s="26"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K58" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11">
       <c r="B59" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" s="4">
         <v>1</v>
@@ -3041,17 +3237,19 @@
         <f t="shared" si="4"/>
         <v>92.660550458715562</v>
       </c>
-      <c r="G59" s="21"/>
-      <c r="H59" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9">
+      <c r="G59" s="26"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11">
       <c r="B60" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C60" s="4">
         <v>4</v>
@@ -3068,17 +3266,19 @@
         <f t="shared" si="4"/>
         <v>96.330275229357767</v>
       </c>
-      <c r="G60" s="21"/>
-      <c r="H60" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="2:9">
+      <c r="G60" s="26"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11">
       <c r="B61" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C61" s="4">
         <v>4</v>
@@ -3095,112 +3295,117 @@
         <f t="shared" si="4"/>
         <v>99.999999999999972</v>
       </c>
-      <c r="G61" s="23"/>
-      <c r="H61" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9">
-      <c r="I62"/>
-    </row>
-    <row r="63" spans="2:9">
-      <c r="I63"/>
-    </row>
-    <row r="64" spans="2:9">
-      <c r="I64"/>
-    </row>
-    <row r="65" spans="9:9">
-      <c r="I65"/>
-    </row>
-    <row r="66" spans="9:9">
-      <c r="I66"/>
-    </row>
-    <row r="67" spans="9:9">
-      <c r="I67"/>
-    </row>
-    <row r="68" spans="9:9">
-      <c r="I68"/>
-    </row>
-    <row r="69" spans="9:9">
-      <c r="I69"/>
-    </row>
-    <row r="70" spans="9:9">
-      <c r="I70"/>
-    </row>
-    <row r="71" spans="9:9">
-      <c r="I71"/>
-    </row>
-    <row r="72" spans="9:9">
-      <c r="I72"/>
-    </row>
-    <row r="73" spans="9:9">
-      <c r="I73"/>
-    </row>
-    <row r="74" spans="9:9">
-      <c r="I74"/>
-    </row>
-    <row r="75" spans="9:9">
-      <c r="I75"/>
-    </row>
-    <row r="76" spans="9:9">
-      <c r="I76"/>
-    </row>
-    <row r="77" spans="9:9">
-      <c r="I77"/>
-    </row>
-    <row r="78" spans="9:9">
-      <c r="I78"/>
-    </row>
-    <row r="79" spans="9:9">
-      <c r="I79"/>
-    </row>
-    <row r="80" spans="9:9">
-      <c r="I80"/>
-    </row>
-    <row r="81" spans="3:9">
-      <c r="I81"/>
-    </row>
-    <row r="82" spans="3:9">
-      <c r="I82"/>
-    </row>
-    <row r="83" spans="3:9">
-      <c r="I83"/>
-    </row>
-    <row r="84" spans="3:9">
+      <c r="G61" s="27"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11">
+      <c r="K62"/>
+    </row>
+    <row r="63" spans="2:11">
+      <c r="K63"/>
+    </row>
+    <row r="64" spans="2:11">
+      <c r="K64"/>
+    </row>
+    <row r="65" spans="11:11">
+      <c r="K65"/>
+    </row>
+    <row r="66" spans="11:11">
+      <c r="K66"/>
+    </row>
+    <row r="67" spans="11:11">
+      <c r="K67"/>
+    </row>
+    <row r="68" spans="11:11">
+      <c r="K68"/>
+    </row>
+    <row r="69" spans="11:11">
+      <c r="K69"/>
+    </row>
+    <row r="70" spans="11:11">
+      <c r="K70"/>
+    </row>
+    <row r="71" spans="11:11">
+      <c r="K71"/>
+    </row>
+    <row r="72" spans="11:11">
+      <c r="K72"/>
+    </row>
+    <row r="73" spans="11:11">
+      <c r="K73"/>
+    </row>
+    <row r="74" spans="11:11">
+      <c r="K74"/>
+    </row>
+    <row r="75" spans="11:11">
+      <c r="K75"/>
+    </row>
+    <row r="76" spans="11:11">
+      <c r="K76"/>
+    </row>
+    <row r="77" spans="11:11">
+      <c r="K77"/>
+    </row>
+    <row r="78" spans="11:11">
+      <c r="K78"/>
+    </row>
+    <row r="79" spans="11:11">
+      <c r="K79"/>
+    </row>
+    <row r="80" spans="11:11">
+      <c r="K80"/>
+    </row>
+    <row r="81" spans="3:11">
+      <c r="K81"/>
+    </row>
+    <row r="82" spans="3:11">
+      <c r="K82"/>
+    </row>
+    <row r="83" spans="3:11">
+      <c r="K83"/>
+    </row>
+    <row r="84" spans="3:11">
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
-      <c r="H84" s="2"/>
-    </row>
-    <row r="85" spans="3:9">
+      <c r="H84" s="3"/>
+      <c r="I84" s="3"/>
+      <c r="J84" s="2"/>
+    </row>
+    <row r="85" spans="3:11">
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="2"/>
-    </row>
-    <row r="86" spans="3:9">
-      <c r="H86" s="1"/>
-      <c r="I86"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="2"/>
+    </row>
+    <row r="86" spans="3:11">
+      <c r="J86" s="1"/>
+      <c r="K86"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="G42:G52"/>
+    <mergeCell ref="G53:G61"/>
     <mergeCell ref="G3:G10"/>
     <mergeCell ref="G11:G15"/>
     <mergeCell ref="G16:G23"/>
     <mergeCell ref="G24:G33"/>
     <mergeCell ref="G34:G41"/>
-    <mergeCell ref="G42:G52"/>
-    <mergeCell ref="G53:G61"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3214,13 +3419,14 @@
   <dimension ref="B4:D14"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B10" sqref="B10:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="42.5" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
@@ -3231,122 +3437,121 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="14">
         <v>1</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="14">
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="14">
         <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="14">
         <v>2</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="14">
         <v>3</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="14">
         <v>2</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="14">
         <v>1</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="14">
         <v>1</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="14">
         <v>1</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3360,14 +3565,14 @@
   <dimension ref="B4:D12"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D12"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:4">
@@ -3378,100 +3583,256 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5">
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="5">
         <v>2</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5">
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="5">
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="5">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D15"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:4">
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="17">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="5">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="5">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Correccion ECU-01, se agrega documento con observaciones
</commit_message>
<xml_diff>
--- a/documentos/General/CronogramaTSP.xlsx
+++ b/documentos/General/CronogramaTSP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="260" windowWidth="25040" windowHeight="14920" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="460" yWindow="260" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma General" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="83">
   <si>
     <t>Tarea</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>Estado</t>
-  </si>
-  <si>
-    <t>TRI</t>
   </si>
   <si>
     <t>Caso de prueba - Modificar propietario</t>
@@ -783,7 +780,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -824,6 +821,12 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -845,25 +848,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1519,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N86"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1533,16 +1518,15 @@
     <col min="5" max="5" width="13.5" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.83203125" customWidth="1"/>
-    <col min="11" max="11" width="18" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1565,16 +1549,13 @@
         <v>78</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
@@ -1593,25 +1574,27 @@
         <f>E3</f>
         <v>1.834862385321101</v>
       </c>
-      <c r="G3" s="28">
-        <v>1</v>
-      </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="G3" s="23">
+        <v>1</v>
+      </c>
+      <c r="H3" s="18">
+        <f>C3*100/$D$61</f>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="L3" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="M3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1630,25 +1613,27 @@
         <f>E4+F3</f>
         <v>5.5045871559633035</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="19">
+        <f t="shared" ref="H4:H61" si="1">C4*100/$D$61</f>
+        <v>3.669724770642202</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="9">
-        <f>SUMIF(J3:J61,"LISTO",E3:E61)</f>
+      <c r="L4" s="9">
+        <f>SUMIF(I3:I61,"LISTO",E3:E61)</f>
         <v>70.642201834862419</v>
       </c>
-      <c r="N4" s="10">
-        <f>100-M4</f>
+      <c r="M4" s="10">
+        <f>100-L4</f>
         <v>29.357798165137581</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1656,7 +1641,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="5">
-        <f t="shared" ref="D5:D22" si="1">D4+C5</f>
+        <f t="shared" ref="D5:D22" si="2">D4+C5</f>
         <v>10</v>
       </c>
       <c r="E5" s="5">
@@ -1664,20 +1649,22 @@
         <v>3.669724770642202</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F22" si="2">E5+F4</f>
+        <f t="shared" ref="F5:F22" si="3">E5+F4</f>
         <v>9.1743119266055047</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="19">
+        <f t="shared" si="1"/>
+        <v>3.669724770642202</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1685,28 +1672,30 @@
         <v>1</v>
       </c>
       <c r="D6" s="5">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="3"/>
+        <v>10.091743119266056</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="19">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F6" s="5">
-        <f t="shared" si="2"/>
-        <v>10.091743119266056</v>
-      </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
@@ -1714,28 +1703,30 @@
         <v>1</v>
       </c>
       <c r="D7" s="5">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="3"/>
+        <v>11.009174311926607</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="19">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="E7" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F7" s="5">
-        <f t="shared" si="2"/>
-        <v>11.009174311926607</v>
-      </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
@@ -1743,28 +1734,30 @@
         <v>1</v>
       </c>
       <c r="D8" s="5">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="3"/>
+        <v>11.926605504587158</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="19">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F8" s="5">
-        <f t="shared" si="2"/>
-        <v>11.926605504587158</v>
-      </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
@@ -1772,28 +1765,30 @@
         <v>1</v>
       </c>
       <c r="D9" s="5">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="3"/>
+        <v>12.844036697247709</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="19">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F9" s="5">
-        <f t="shared" si="2"/>
-        <v>12.844036697247709</v>
-      </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:13">
       <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
@@ -1801,28 +1796,30 @@
         <v>1</v>
       </c>
       <c r="D10" s="5">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="3"/>
+        <v>13.761467889908261</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="19">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F10" s="5">
-        <f t="shared" si="2"/>
-        <v>13.761467889908261</v>
-      </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:13">
       <c r="B11" s="7" t="s">
         <v>36</v>
       </c>
@@ -1830,30 +1827,32 @@
         <v>2</v>
       </c>
       <c r="D11" s="5">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="3"/>
+        <v>15.596330275229361</v>
+      </c>
+      <c r="G11" s="23">
+        <v>2</v>
+      </c>
+      <c r="H11" s="19">
         <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="E11" s="5">
-        <f t="shared" si="0"/>
         <v>1.834862385321101</v>
       </c>
-      <c r="F11" s="5">
-        <f t="shared" si="2"/>
-        <v>15.596330275229361</v>
-      </c>
-      <c r="G11" s="28">
-        <v>2</v>
-      </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="I11" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:13">
       <c r="B12" s="7" t="s">
         <v>37</v>
       </c>
@@ -1861,28 +1860,30 @@
         <v>3</v>
       </c>
       <c r="D12" s="5">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7522935779816513</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="3"/>
+        <v>18.348623853211013</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="19">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="E12" s="5">
-        <f t="shared" si="0"/>
         <v>2.7522935779816513</v>
       </c>
-      <c r="F12" s="5">
-        <f t="shared" si="2"/>
-        <v>18.348623853211013</v>
-      </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
+      <c r="I12" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:13">
       <c r="B13" s="7" t="s">
         <v>38</v>
       </c>
@@ -1890,28 +1891,30 @@
         <v>1</v>
       </c>
       <c r="D13" s="5">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="3"/>
+        <v>19.266055045871564</v>
+      </c>
+      <c r="G13" s="23"/>
+      <c r="H13" s="19">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="E13" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F13" s="5">
-        <f t="shared" si="2"/>
-        <v>19.266055045871564</v>
-      </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:13">
       <c r="B14" s="7" t="s">
         <v>32</v>
       </c>
@@ -1919,28 +1922,30 @@
         <v>1</v>
       </c>
       <c r="D14" s="5">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="3"/>
+        <v>20.183486238532115</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="19">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="E14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F14" s="5">
-        <f t="shared" si="2"/>
-        <v>20.183486238532115</v>
-      </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:13">
       <c r="B15" s="7" t="s">
         <v>33</v>
       </c>
@@ -1948,28 +1953,30 @@
         <v>8</v>
       </c>
       <c r="D15" s="5">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>7.3394495412844041</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="3"/>
+        <v>27.522935779816521</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="19">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="E15" s="5">
-        <f t="shared" si="0"/>
         <v>7.3394495412844041</v>
       </c>
-      <c r="F15" s="5">
-        <f t="shared" si="2"/>
-        <v>27.522935779816521</v>
-      </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="I15" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:13">
       <c r="A16" s="2"/>
       <c r="B16" s="8" t="s">
         <v>34</v>
@@ -1978,30 +1985,32 @@
         <v>3</v>
       </c>
       <c r="D16" s="5">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7522935779816513</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="3"/>
+        <v>30.275229357798171</v>
+      </c>
+      <c r="G16" s="23">
+        <v>3</v>
+      </c>
+      <c r="H16" s="19">
         <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="E16" s="5">
-        <f t="shared" si="0"/>
         <v>2.7522935779816513</v>
       </c>
-      <c r="F16" s="5">
-        <f t="shared" si="2"/>
-        <v>30.275229357798171</v>
-      </c>
-      <c r="G16" s="28">
-        <v>3</v>
-      </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="I16" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:10">
       <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
@@ -2009,28 +2018,30 @@
         <v>1</v>
       </c>
       <c r="D17" s="5">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="3"/>
+        <v>31.192660550458722</v>
+      </c>
+      <c r="G17" s="23"/>
+      <c r="H17" s="19">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="E17" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F17" s="5">
-        <f t="shared" si="2"/>
-        <v>31.192660550458722</v>
-      </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K17" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:10">
       <c r="B18" s="7" t="s">
         <v>13</v>
       </c>
@@ -2038,28 +2049,30 @@
         <v>1</v>
       </c>
       <c r="D18" s="5">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="3"/>
+        <v>32.11009174311927</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="19">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="E18" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F18" s="5">
-        <f t="shared" si="2"/>
-        <v>32.11009174311927</v>
-      </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:10">
       <c r="B19" s="7" t="s">
         <v>11</v>
       </c>
@@ -2067,28 +2080,30 @@
         <v>1</v>
       </c>
       <c r="D19" s="5">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="3"/>
+        <v>33.027522935779821</v>
+      </c>
+      <c r="G19" s="23"/>
+      <c r="H19" s="19">
         <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="E19" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F19" s="5">
-        <f t="shared" si="2"/>
-        <v>33.027522935779821</v>
-      </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:10">
       <c r="B20" s="7" t="s">
         <v>28</v>
       </c>
@@ -2096,28 +2111,30 @@
         <v>1</v>
       </c>
       <c r="D20" s="5">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="3"/>
+        <v>33.944954128440372</v>
+      </c>
+      <c r="G20" s="23"/>
+      <c r="H20" s="19">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="E20" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F20" s="5">
-        <f t="shared" si="2"/>
-        <v>33.944954128440372</v>
-      </c>
-      <c r="G20" s="28"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:10">
       <c r="B21" s="7" t="s">
         <v>39</v>
       </c>
@@ -2125,28 +2142,30 @@
         <v>1</v>
       </c>
       <c r="D21" s="5">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="3"/>
+        <v>34.862385321100923</v>
+      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="19">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="E21" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91743119266055051</v>
-      </c>
-      <c r="F21" s="5">
-        <f t="shared" si="2"/>
-        <v>34.862385321100923</v>
-      </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K21" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:10">
       <c r="B22" s="7" t="s">
         <v>37</v>
       </c>
@@ -2154,28 +2173,30 @@
         <v>4</v>
       </c>
       <c r="D22" s="5">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>3.669724770642202</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="3"/>
+        <v>38.532110091743128</v>
+      </c>
+      <c r="G22" s="23"/>
+      <c r="H22" s="19">
         <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="E22" s="5">
-        <f t="shared" si="0"/>
         <v>3.669724770642202</v>
       </c>
-      <c r="F22" s="5">
-        <f t="shared" si="2"/>
-        <v>38.532110091743128</v>
-      </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
+      <c r="I22" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:10">
       <c r="B23" s="7" t="s">
         <v>31</v>
       </c>
@@ -2194,17 +2215,19 @@
         <f>E23+F22</f>
         <v>41.284403669724782</v>
       </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="19">
+        <f t="shared" si="1"/>
+        <v>2.7522935779816513</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K23" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:10">
       <c r="B24" s="12" t="s">
         <v>46</v>
       </c>
@@ -2212,7 +2235,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" ref="D24:D61" si="3">D23+C24</f>
+        <f t="shared" ref="D24:D61" si="4">D23+C24</f>
         <v>46</v>
       </c>
       <c r="E24" s="5">
@@ -2220,22 +2243,24 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" ref="F24:F61" si="4">E24+F23</f>
+        <f t="shared" ref="F24:F61" si="5">E24+F23</f>
         <v>42.201834862385333</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="24">
         <v>4</v>
       </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K24" s="14" t="s">
+      <c r="H24" s="19">
+        <f t="shared" si="1"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:10">
       <c r="B25" s="13" t="s">
         <v>47</v>
       </c>
@@ -2243,7 +2268,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>47</v>
       </c>
       <c r="E25" s="5">
@@ -2251,20 +2276,22 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43.119266055045884</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K25" s="14" t="s">
+      <c r="G25" s="25"/>
+      <c r="H25" s="19">
+        <f t="shared" si="1"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:10">
       <c r="B26" s="13" t="s">
         <v>48</v>
       </c>
@@ -2272,7 +2299,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
       <c r="E26" s="5">
@@ -2280,20 +2307,22 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44.036697247706435</v>
       </c>
-      <c r="G26" s="30"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K26" s="14" t="s">
+      <c r="G26" s="25"/>
+      <c r="H26" s="19">
+        <f t="shared" si="1"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:10">
       <c r="B27" s="13" t="s">
         <v>49</v>
       </c>
@@ -2301,7 +2330,7 @@
         <v>2</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="E27" s="5">
@@ -2309,20 +2338,22 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F27" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45.871559633027537</v>
       </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K27" s="14" t="s">
+      <c r="G27" s="25"/>
+      <c r="H27" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:10">
       <c r="B28" s="13" t="s">
         <v>50</v>
       </c>
@@ -2330,7 +2361,7 @@
         <v>3</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="E28" s="5">
@@ -2338,20 +2369,22 @@
         <v>2.7522935779816513</v>
       </c>
       <c r="F28" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>48.623853211009191</v>
       </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K28" s="14" t="s">
+      <c r="G28" s="25"/>
+      <c r="H28" s="19">
+        <f t="shared" si="1"/>
+        <v>2.7522935779816513</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:11">
+    <row r="29" spans="2:10">
       <c r="B29" s="13" t="s">
         <v>51</v>
       </c>
@@ -2359,7 +2392,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="E29" s="5">
@@ -2367,20 +2400,22 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F29" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>50.458715596330293</v>
       </c>
-      <c r="G29" s="30"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K29" s="14" t="s">
+      <c r="G29" s="25"/>
+      <c r="H29" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:11">
+    <row r="30" spans="2:10">
       <c r="B30" s="13" t="s">
         <v>52</v>
       </c>
@@ -2388,7 +2423,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="E30" s="5">
@@ -2396,20 +2431,22 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F30" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51.376146788990845</v>
       </c>
-      <c r="G30" s="30"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K30" s="14" t="s">
+      <c r="G30" s="25"/>
+      <c r="H30" s="19">
+        <f t="shared" si="1"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:11">
+    <row r="31" spans="2:10">
       <c r="B31" s="13" t="s">
         <v>53</v>
       </c>
@@ -2417,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="E31" s="5">
@@ -2425,20 +2462,22 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>52.293577981651396</v>
       </c>
-      <c r="G31" s="30"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K31" s="14" t="s">
+      <c r="G31" s="25"/>
+      <c r="H31" s="19">
+        <f t="shared" si="1"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="14" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="2:11">
+    <row r="32" spans="2:10">
       <c r="B32" s="13" t="s">
         <v>54</v>
       </c>
@@ -2446,7 +2485,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="E32" s="5">
@@ -2454,20 +2493,22 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F32" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>53.211009174311947</v>
       </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" s="14" t="s">
+      <c r="G32" s="25"/>
+      <c r="H32" s="19">
+        <f t="shared" si="1"/>
+        <v>0.91743119266055051</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="2:10">
       <c r="B33" s="13" t="s">
         <v>29</v>
       </c>
@@ -2475,7 +2516,7 @@
         <v>3</v>
       </c>
       <c r="D33" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="E33" s="5">
@@ -2483,20 +2524,22 @@
         <v>2.7522935779816513</v>
       </c>
       <c r="F33" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>55.9633027522936</v>
       </c>
-      <c r="G33" s="31"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K33" s="14" t="s">
+      <c r="G33" s="26"/>
+      <c r="H33" s="19">
+        <f t="shared" si="1"/>
+        <v>2.7522935779816513</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="2:11">
+    <row r="34" spans="2:10">
       <c r="B34" s="7" t="s">
         <v>25</v>
       </c>
@@ -2504,7 +2547,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="E34" s="5">
@@ -2512,22 +2555,24 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F34" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>57.798165137614703</v>
       </c>
-      <c r="G34" s="29">
+      <c r="G34" s="24">
         <v>5</v>
       </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
+      <c r="H34" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J34" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K34" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:11">
+    <row r="35" spans="2:10">
       <c r="B35" s="7" t="s">
         <v>26</v>
       </c>
@@ -2535,7 +2580,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="E35" s="5">
@@ -2543,20 +2588,22 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F35" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.633027522935805</v>
       </c>
-      <c r="G35" s="30"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K35" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="2:11">
+    <row r="36" spans="2:10">
       <c r="B36" s="7" t="s">
         <v>58</v>
       </c>
@@ -2564,7 +2611,7 @@
         <v>2</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="E36" s="5">
@@ -2572,20 +2619,22 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F36" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>61.467889908256907</v>
       </c>
-      <c r="G36" s="30"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K36" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="2:11">
+    <row r="37" spans="2:10">
       <c r="B37" s="7" t="s">
         <v>14</v>
       </c>
@@ -2593,7 +2642,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="E37" s="5">
@@ -2601,20 +2650,22 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F37" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>63.30275229357801</v>
       </c>
-      <c r="G37" s="30"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K37" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="2:11">
+    <row r="38" spans="2:10">
       <c r="B38" s="7" t="s">
         <v>15</v>
       </c>
@@ -2622,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="E38" s="5">
@@ -2630,20 +2681,22 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F38" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>65.137614678899112</v>
       </c>
-      <c r="G38" s="30"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J38" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K38" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="2:11">
+    <row r="39" spans="2:10">
       <c r="B39" s="7" t="s">
         <v>16</v>
       </c>
@@ -2651,7 +2704,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="E39" s="5">
@@ -2659,20 +2712,22 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F39" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66.972477064220215</v>
       </c>
-      <c r="G39" s="30"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J39" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K39" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="2:11">
+    <row r="40" spans="2:10">
       <c r="B40" s="7" t="s">
         <v>56</v>
       </c>
@@ -2680,7 +2735,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="E40" s="5">
@@ -2688,20 +2743,22 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F40" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68.807339449541317</v>
       </c>
-      <c r="G40" s="30"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J40" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K40" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="2:11">
+    <row r="41" spans="2:10">
       <c r="B41" s="7" t="s">
         <v>57</v>
       </c>
@@ -2709,7 +2766,7 @@
         <v>2</v>
       </c>
       <c r="D41" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
       <c r="E41" s="5">
@@ -2717,20 +2774,22 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F41" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>70.642201834862419</v>
       </c>
-      <c r="G41" s="31"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="19">
+        <f t="shared" si="1"/>
+        <v>1.834862385321101</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J41" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K41" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="2:11">
+    <row r="42" spans="2:10">
       <c r="B42" s="13" t="s">
         <v>59</v>
       </c>
@@ -2738,7 +2797,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
       <c r="E42" s="4">
@@ -2746,22 +2805,21 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.559633027522963</v>
       </c>
-      <c r="G42" s="25">
+      <c r="G42" s="20">
         <v>6</v>
       </c>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J42" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K42" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="2:11">
+    <row r="43" spans="2:10">
       <c r="B43" s="13" t="s">
         <v>60</v>
       </c>
@@ -2769,7 +2827,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>79</v>
       </c>
       <c r="E43" s="4">
@@ -2777,20 +2835,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F43" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.477064220183507</v>
       </c>
-      <c r="G43" s="26"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J43" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K43" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="2:11">
+    <row r="44" spans="2:10">
       <c r="B44" s="7" t="s">
         <v>61</v>
       </c>
@@ -2798,7 +2855,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="E44" s="4">
@@ -2806,20 +2863,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F44" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.394495412844051</v>
       </c>
-      <c r="G44" s="26"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J44" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K44" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="2:11">
+    <row r="45" spans="2:10">
       <c r="B45" s="7" t="s">
         <v>62</v>
       </c>
@@ -2827,7 +2883,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>81</v>
       </c>
       <c r="E45" s="4">
@@ -2835,20 +2891,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F45" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.311926605504595</v>
       </c>
-      <c r="G45" s="26"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J45" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K45" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="2:11">
+    <row r="46" spans="2:10">
       <c r="B46" s="7" t="s">
         <v>63</v>
       </c>
@@ -2856,7 +2911,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82</v>
       </c>
       <c r="E46" s="4">
@@ -2864,20 +2919,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F46" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.22935779816514</v>
       </c>
-      <c r="G46" s="26"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J46" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K46" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="2:11">
+    <row r="47" spans="2:10">
       <c r="B47" s="7" t="s">
         <v>64</v>
       </c>
@@ -2885,7 +2939,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83</v>
       </c>
       <c r="E47" s="4">
@@ -2893,20 +2947,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F47" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>76.146788990825684</v>
       </c>
-      <c r="G47" s="26"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J47" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K47" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="2:11">
+    <row r="48" spans="2:10">
       <c r="B48" s="7" t="s">
         <v>65</v>
       </c>
@@ -2914,7 +2967,7 @@
         <v>2</v>
       </c>
       <c r="D48" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
       <c r="E48" s="4">
@@ -2922,20 +2975,19 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F48" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>77.981651376146786</v>
       </c>
-      <c r="G48" s="26"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J48" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K48" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="2:11">
+    <row r="49" spans="2:10">
       <c r="B49" s="7" t="s">
         <v>66</v>
       </c>
@@ -2943,7 +2995,7 @@
         <v>2</v>
       </c>
       <c r="D49" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87</v>
       </c>
       <c r="E49" s="4">
@@ -2951,20 +3003,19 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F49" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79.816513761467888</v>
       </c>
-      <c r="G49" s="26"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J49" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K49" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="2:11">
+    <row r="50" spans="2:10">
       <c r="B50" s="7" t="s">
         <v>67</v>
       </c>
@@ -2972,7 +3023,7 @@
         <v>2</v>
       </c>
       <c r="D50" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89</v>
       </c>
       <c r="E50" s="4">
@@ -2980,20 +3031,19 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F50" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>81.651376146788991</v>
       </c>
-      <c r="G50" s="26"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J50" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K50" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="2:11">
+    <row r="51" spans="2:10">
       <c r="B51" s="7" t="s">
         <v>68</v>
       </c>
@@ -3001,7 +3051,7 @@
         <v>2</v>
       </c>
       <c r="D51" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
       <c r="E51" s="4">
@@ -3009,20 +3059,19 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F51" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83.486238532110093</v>
       </c>
-      <c r="G51" s="26"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J51" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K51" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="2:11">
+    <row r="52" spans="2:10">
       <c r="B52" s="7" t="s">
         <v>69</v>
       </c>
@@ -3030,7 +3079,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>93</v>
       </c>
       <c r="E52" s="4">
@@ -3038,20 +3087,19 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F52" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>85.321100917431195</v>
       </c>
-      <c r="G52" s="26"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J52" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K52" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="2:11">
+    <row r="53" spans="2:10">
       <c r="B53" s="7" t="s">
         <v>70</v>
       </c>
@@ -3059,7 +3107,7 @@
         <v>2</v>
       </c>
       <c r="D53" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
       <c r="E53" s="4">
@@ -3067,22 +3115,21 @@
         <v>1.834862385321101</v>
       </c>
       <c r="F53" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>87.155963302752298</v>
       </c>
-      <c r="G53" s="25">
+      <c r="G53" s="20">
         <v>7</v>
       </c>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J53" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K53" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="2:11">
+    <row r="54" spans="2:10">
       <c r="B54" s="7" t="s">
         <v>71</v>
       </c>
@@ -3090,7 +3137,7 @@
         <v>1</v>
       </c>
       <c r="D54" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
       <c r="E54" s="4">
@@ -3098,20 +3145,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F54" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>88.073394495412842</v>
       </c>
-      <c r="G54" s="26"/>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="4" t="s">
+      <c r="G54" s="21"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K54" s="16" t="s">
+      <c r="J54" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="2:11">
+    <row r="55" spans="2:10">
       <c r="B55" s="7" t="s">
         <v>72</v>
       </c>
@@ -3119,7 +3165,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
       <c r="E55" s="4">
@@ -3127,20 +3173,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F55" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>88.990825688073386</v>
       </c>
-      <c r="G55" s="26"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J55" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K55" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="2:11">
+    <row r="56" spans="2:10">
       <c r="B56" s="7" t="s">
         <v>73</v>
       </c>
@@ -3148,7 +3193,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
       <c r="E56" s="4">
@@ -3156,20 +3201,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F56" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>89.90825688073393</v>
       </c>
-      <c r="G56" s="26"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J56" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K56" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="2:11">
+    <row r="57" spans="2:10">
       <c r="B57" s="7" t="s">
         <v>74</v>
       </c>
@@ -3177,7 +3221,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
       <c r="E57" s="4">
@@ -3185,20 +3229,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F57" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90.825688073394474</v>
       </c>
-      <c r="G57" s="26"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J57" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K57" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="2:11">
+    <row r="58" spans="2:10">
       <c r="B58" s="7" t="s">
         <v>75</v>
       </c>
@@ -3206,7 +3249,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="E58" s="4">
@@ -3214,20 +3257,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F58" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>91.743119266055018</v>
       </c>
-      <c r="G58" s="26"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="4" t="s">
+      <c r="G58" s="21"/>
+      <c r="H58" s="27"/>
+      <c r="I58" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K58" s="16" t="s">
+      <c r="J58" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="2:11">
+    <row r="59" spans="2:10">
       <c r="B59" s="7" t="s">
         <v>76</v>
       </c>
@@ -3235,7 +3277,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
       <c r="E59" s="4">
@@ -3243,20 +3285,19 @@
         <v>0.91743119266055051</v>
       </c>
       <c r="F59" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>92.660550458715562</v>
       </c>
-      <c r="G59" s="26"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J59" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K59" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="2:11">
+    <row r="60" spans="2:10">
       <c r="B60" s="7" t="s">
         <v>30</v>
       </c>
@@ -3264,7 +3305,7 @@
         <v>4</v>
       </c>
       <c r="D60" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>105</v>
       </c>
       <c r="E60" s="4">
@@ -3272,20 +3313,19 @@
         <v>3.669724770642202</v>
       </c>
       <c r="F60" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>96.330275229357767</v>
       </c>
-      <c r="G60" s="26"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="27"/>
+      <c r="I60" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J60" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K60" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="2:11">
+    <row r="61" spans="2:10">
       <c r="B61" s="7" t="s">
         <v>40</v>
       </c>
@@ -3293,7 +3333,7 @@
         <v>4</v>
       </c>
       <c r="D61" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>109</v>
       </c>
       <c r="E61" s="4">
@@ -3301,108 +3341,105 @@
         <v>3.669724770642202</v>
       </c>
       <c r="F61" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>99.999999999999972</v>
       </c>
-      <c r="G61" s="27"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="J61" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K61" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="2:11">
-      <c r="K62"/>
-    </row>
-    <row r="63" spans="2:11">
-      <c r="K63"/>
-    </row>
-    <row r="64" spans="2:11">
-      <c r="K64"/>
-    </row>
-    <row r="65" spans="11:11">
-      <c r="K65"/>
-    </row>
-    <row r="66" spans="11:11">
-      <c r="K66"/>
-    </row>
-    <row r="67" spans="11:11">
-      <c r="K67"/>
-    </row>
-    <row r="68" spans="11:11">
-      <c r="K68"/>
-    </row>
-    <row r="69" spans="11:11">
-      <c r="K69"/>
-    </row>
-    <row r="70" spans="11:11">
-      <c r="K70"/>
-    </row>
-    <row r="71" spans="11:11">
-      <c r="K71"/>
-    </row>
-    <row r="72" spans="11:11">
-      <c r="K72"/>
-    </row>
-    <row r="73" spans="11:11">
-      <c r="K73"/>
-    </row>
-    <row r="74" spans="11:11">
-      <c r="K74"/>
-    </row>
-    <row r="75" spans="11:11">
-      <c r="K75"/>
-    </row>
-    <row r="76" spans="11:11">
-      <c r="K76"/>
-    </row>
-    <row r="77" spans="11:11">
-      <c r="K77"/>
-    </row>
-    <row r="78" spans="11:11">
-      <c r="K78"/>
-    </row>
-    <row r="79" spans="11:11">
-      <c r="K79"/>
-    </row>
-    <row r="80" spans="11:11">
-      <c r="K80"/>
-    </row>
-    <row r="81" spans="3:11">
-      <c r="K81"/>
-    </row>
-    <row r="82" spans="3:11">
-      <c r="K82"/>
-    </row>
-    <row r="83" spans="3:11">
-      <c r="K83"/>
-    </row>
-    <row r="84" spans="3:11">
+    <row r="62" spans="2:10">
+      <c r="J62"/>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="J63"/>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="J64"/>
+    </row>
+    <row r="65" spans="10:10">
+      <c r="J65"/>
+    </row>
+    <row r="66" spans="10:10">
+      <c r="J66"/>
+    </row>
+    <row r="67" spans="10:10">
+      <c r="J67"/>
+    </row>
+    <row r="68" spans="10:10">
+      <c r="J68"/>
+    </row>
+    <row r="69" spans="10:10">
+      <c r="J69"/>
+    </row>
+    <row r="70" spans="10:10">
+      <c r="J70"/>
+    </row>
+    <row r="71" spans="10:10">
+      <c r="J71"/>
+    </row>
+    <row r="72" spans="10:10">
+      <c r="J72"/>
+    </row>
+    <row r="73" spans="10:10">
+      <c r="J73"/>
+    </row>
+    <row r="74" spans="10:10">
+      <c r="J74"/>
+    </row>
+    <row r="75" spans="10:10">
+      <c r="J75"/>
+    </row>
+    <row r="76" spans="10:10">
+      <c r="J76"/>
+    </row>
+    <row r="77" spans="10:10">
+      <c r="J77"/>
+    </row>
+    <row r="78" spans="10:10">
+      <c r="J78"/>
+    </row>
+    <row r="79" spans="10:10">
+      <c r="J79"/>
+    </row>
+    <row r="80" spans="10:10">
+      <c r="J80"/>
+    </row>
+    <row r="81" spans="3:10">
+      <c r="J81"/>
+    </row>
+    <row r="82" spans="3:10">
+      <c r="J82"/>
+    </row>
+    <row r="83" spans="3:10">
+      <c r="J83"/>
+    </row>
+    <row r="84" spans="3:10">
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-      <c r="J84" s="2"/>
-    </row>
-    <row r="85" spans="3:11">
+      <c r="I84" s="2"/>
+    </row>
+    <row r="85" spans="3:10">
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
-      <c r="J85" s="2"/>
-    </row>
-    <row r="86" spans="3:11">
-      <c r="J86" s="1"/>
-      <c r="K86"/>
+      <c r="I85" s="2"/>
+    </row>
+    <row r="86" spans="3:10">
+      <c r="I86" s="1"/>
+      <c r="J86"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3428,7 +3465,7 @@
   <dimension ref="B4:D14"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3457,7 +3494,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -3517,7 +3554,7 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" s="14">
         <v>1</v>
@@ -3528,18 +3565,18 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="14">
         <v>1</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="14">
         <v>1</v>
@@ -3556,7 +3593,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -3697,8 +3734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Check-ECU-07, ECU-07 y cronograma
</commit_message>
<xml_diff>
--- a/documentos/General/CronogramaTSP.xlsx
+++ b/documentos/General/CronogramaTSP.xlsx
@@ -410,8 +410,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="347">
+  <cellStyleXfs count="361">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -803,6 +817,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -815,20 +841,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="347">
+  <cellStyles count="361">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1002,6 +1016,13 @@
     <cellStyle name="Hipervínculo" xfId="341" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="343" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="359" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -1175,6 +1196,13 @@
     <cellStyle name="Hipervínculo visitado" xfId="342" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="344" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="360" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1506,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1574,7 +1602,7 @@
         <f>E3</f>
         <v>2.1739130434782608</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="23">
         <v>1</v>
       </c>
       <c r="H3" s="16">
@@ -1613,7 +1641,7 @@
         <f>E4+F3</f>
         <v>6.5217391304347823</v>
       </c>
-      <c r="G4" s="19"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="17">
         <f t="shared" ref="H4:H41" si="1">C4*100/$D$52</f>
         <v>4.3478260869565215</v>
@@ -1652,7 +1680,7 @@
         <f t="shared" ref="F5:F22" si="3">E5+F4</f>
         <v>10.869565217391305</v>
       </c>
-      <c r="G5" s="19"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="17">
         <f t="shared" si="1"/>
         <v>4.3478260869565215</v>
@@ -1683,7 +1711,7 @@
         <f t="shared" si="3"/>
         <v>11.956521739130435</v>
       </c>
-      <c r="G6" s="19"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -1714,7 +1742,7 @@
         <f t="shared" si="3"/>
         <v>13.043478260869566</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -1745,7 +1773,7 @@
         <f t="shared" si="3"/>
         <v>14.130434782608697</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -1776,7 +1804,7 @@
         <f t="shared" si="3"/>
         <v>15.217391304347828</v>
       </c>
-      <c r="G9" s="19"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -1807,7 +1835,7 @@
         <f t="shared" si="3"/>
         <v>16.304347826086957</v>
       </c>
-      <c r="G10" s="19"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -1838,7 +1866,7 @@
         <f t="shared" si="3"/>
         <v>18.478260869565219</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="23">
         <v>2</v>
       </c>
       <c r="H11" s="17">
@@ -1871,7 +1899,7 @@
         <f t="shared" si="3"/>
         <v>21.739130434782609</v>
       </c>
-      <c r="G12" s="19"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="17">
         <f t="shared" si="1"/>
         <v>3.2608695652173911</v>
@@ -1902,7 +1930,7 @@
         <f t="shared" si="3"/>
         <v>22.826086956521738</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -1933,7 +1961,7 @@
         <f t="shared" si="3"/>
         <v>23.913043478260867</v>
       </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="23"/>
       <c r="H14" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -1964,7 +1992,7 @@
         <f t="shared" si="3"/>
         <v>32.608695652173907</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="23"/>
       <c r="H15" s="17">
         <f t="shared" si="1"/>
         <v>8.695652173913043</v>
@@ -1996,7 +2024,7 @@
         <f t="shared" si="3"/>
         <v>35.869565217391298</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="23">
         <v>3</v>
       </c>
       <c r="H16" s="17">
@@ -2029,7 +2057,7 @@
         <f t="shared" si="3"/>
         <v>36.95652173913043</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2060,7 +2088,7 @@
         <f t="shared" si="3"/>
         <v>38.043478260869563</v>
       </c>
-      <c r="G18" s="19"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2091,7 +2119,7 @@
         <f t="shared" si="3"/>
         <v>39.130434782608695</v>
       </c>
-      <c r="G19" s="19"/>
+      <c r="G19" s="23"/>
       <c r="H19" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2122,7 +2150,7 @@
         <f t="shared" si="3"/>
         <v>40.217391304347828</v>
       </c>
-      <c r="G20" s="19"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2153,7 +2181,7 @@
         <f t="shared" si="3"/>
         <v>41.304347826086961</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2184,7 +2212,7 @@
         <f t="shared" si="3"/>
         <v>45.652173913043484</v>
       </c>
-      <c r="G22" s="19"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="17">
         <f t="shared" si="1"/>
         <v>4.3478260869565215</v>
@@ -2215,7 +2243,7 @@
         <f>E23+F22</f>
         <v>48.913043478260875</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="23"/>
       <c r="H23" s="17">
         <f t="shared" si="1"/>
         <v>3.2608695652173911</v>
@@ -2246,7 +2274,7 @@
         <f t="shared" ref="F24:F52" si="5">E24+F23</f>
         <v>50.000000000000007</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G24" s="24">
         <v>4</v>
       </c>
       <c r="H24" s="17">
@@ -2279,7 +2307,7 @@
         <f t="shared" si="5"/>
         <v>51.08695652173914</v>
       </c>
-      <c r="G25" s="21"/>
+      <c r="G25" s="25"/>
       <c r="H25" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2310,7 +2338,7 @@
         <f t="shared" si="5"/>
         <v>52.173913043478272</v>
       </c>
-      <c r="G26" s="21"/>
+      <c r="G26" s="25"/>
       <c r="H26" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2341,7 +2369,7 @@
         <f t="shared" si="5"/>
         <v>54.34782608695653</v>
       </c>
-      <c r="G27" s="21"/>
+      <c r="G27" s="25"/>
       <c r="H27" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2372,7 +2400,7 @@
         <f t="shared" si="5"/>
         <v>57.608695652173921</v>
       </c>
-      <c r="G28" s="21"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="17">
         <f t="shared" si="1"/>
         <v>3.2608695652173911</v>
@@ -2403,7 +2431,7 @@
         <f t="shared" si="5"/>
         <v>59.782608695652179</v>
       </c>
-      <c r="G29" s="21"/>
+      <c r="G29" s="25"/>
       <c r="H29" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2434,7 +2462,7 @@
         <f t="shared" si="5"/>
         <v>60.869565217391312</v>
       </c>
-      <c r="G30" s="21"/>
+      <c r="G30" s="25"/>
       <c r="H30" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2465,7 +2493,7 @@
         <f t="shared" si="5"/>
         <v>61.956521739130444</v>
       </c>
-      <c r="G31" s="21"/>
+      <c r="G31" s="25"/>
       <c r="H31" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2496,7 +2524,7 @@
         <f t="shared" si="5"/>
         <v>63.043478260869577</v>
       </c>
-      <c r="G32" s="21"/>
+      <c r="G32" s="25"/>
       <c r="H32" s="17">
         <f t="shared" si="1"/>
         <v>1.0869565217391304</v>
@@ -2527,7 +2555,7 @@
         <f t="shared" si="5"/>
         <v>65.217391304347842</v>
       </c>
-      <c r="G33" s="22"/>
+      <c r="G33" s="26"/>
       <c r="H33" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2558,7 +2586,7 @@
         <f t="shared" si="5"/>
         <v>67.391304347826107</v>
       </c>
-      <c r="G34" s="20">
+      <c r="G34" s="24">
         <v>5</v>
       </c>
       <c r="H34" s="17">
@@ -2591,7 +2619,7 @@
         <f t="shared" si="5"/>
         <v>69.565217391304373</v>
       </c>
-      <c r="G35" s="21"/>
+      <c r="G35" s="25"/>
       <c r="H35" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2622,7 +2650,7 @@
         <f t="shared" si="5"/>
         <v>71.739130434782638</v>
       </c>
-      <c r="G36" s="21"/>
+      <c r="G36" s="25"/>
       <c r="H36" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2653,7 +2681,7 @@
         <f t="shared" si="5"/>
         <v>73.913043478260903</v>
       </c>
-      <c r="G37" s="21"/>
+      <c r="G37" s="25"/>
       <c r="H37" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2684,7 +2712,7 @@
         <f t="shared" si="5"/>
         <v>76.086956521739168</v>
       </c>
-      <c r="G38" s="21"/>
+      <c r="G38" s="25"/>
       <c r="H38" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2715,7 +2743,7 @@
         <f t="shared" si="5"/>
         <v>78.260869565217433</v>
       </c>
-      <c r="G39" s="21"/>
+      <c r="G39" s="25"/>
       <c r="H39" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2746,7 +2774,7 @@
         <f t="shared" si="5"/>
         <v>80.434782608695699</v>
       </c>
-      <c r="G40" s="21"/>
+      <c r="G40" s="25"/>
       <c r="H40" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2777,7 +2805,7 @@
         <f t="shared" si="5"/>
         <v>82.608695652173964</v>
       </c>
-      <c r="G41" s="22"/>
+      <c r="G41" s="26"/>
       <c r="H41" s="17">
         <f t="shared" si="1"/>
         <v>2.1739130434782608</v>
@@ -2808,7 +2836,7 @@
         <f t="shared" si="5"/>
         <v>83.695652173913089</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G42" s="22">
         <v>6</v>
       </c>
       <c r="H42" s="18" t="s">
@@ -2817,7 +2845,7 @@
       <c r="I42" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J42" s="25" t="s">
+      <c r="J42" s="20" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2840,14 +2868,14 @@
         <f t="shared" si="5"/>
         <v>84.782608695652215</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="22"/>
       <c r="H43" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J43" s="26" t="s">
+      <c r="J43" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2870,14 +2898,14 @@
         <f t="shared" si="5"/>
         <v>85.86956521739134</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="22"/>
       <c r="H44" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J44" s="26" t="s">
+      <c r="J44" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2900,14 +2928,14 @@
         <f t="shared" si="5"/>
         <v>86.956521739130466</v>
       </c>
-      <c r="G45" s="24"/>
+      <c r="G45" s="22"/>
       <c r="H45" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J45" s="26" t="s">
+      <c r="J45" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2930,14 +2958,14 @@
         <f t="shared" si="5"/>
         <v>88.043478260869591</v>
       </c>
-      <c r="G46" s="24"/>
-      <c r="H46" s="23" t="s">
+      <c r="G46" s="22"/>
+      <c r="H46" s="19" t="s">
         <v>42</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J46" s="26" t="s">
+      <c r="J46" s="21" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2960,14 +2988,14 @@
         <f t="shared" si="5"/>
         <v>89.130434782608717</v>
       </c>
-      <c r="G47" s="24"/>
+      <c r="G47" s="22"/>
       <c r="H47" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J47" s="26" t="s">
+      <c r="J47" s="21" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2990,14 +3018,14 @@
         <f t="shared" si="5"/>
         <v>91.304347826086982</v>
       </c>
-      <c r="G48" s="24"/>
+      <c r="G48" s="22"/>
       <c r="H48" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J48" s="26" t="s">
+      <c r="J48" s="21" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3020,14 +3048,14 @@
         <f t="shared" si="5"/>
         <v>93.478260869565247</v>
       </c>
-      <c r="G49" s="24"/>
+      <c r="G49" s="22"/>
       <c r="H49" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J49" s="26" t="s">
+      <c r="J49" s="21" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3050,14 +3078,14 @@
         <f t="shared" si="5"/>
         <v>95.652173913043512</v>
       </c>
-      <c r="G50" s="24"/>
+      <c r="G50" s="22"/>
       <c r="H50" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J50" s="26" t="s">
+      <c r="J50" s="21" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3080,14 +3108,14 @@
         <f t="shared" si="5"/>
         <v>97.826086956521777</v>
       </c>
-      <c r="G51" s="24"/>
+      <c r="G51" s="22"/>
       <c r="H51" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J51" s="26" t="s">
+      <c r="J51" s="21" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3110,14 +3138,14 @@
         <f t="shared" si="5"/>
         <v>100.00000000000004</v>
       </c>
-      <c r="G52" s="24"/>
+      <c r="G52" s="22"/>
       <c r="H52" s="18" t="s">
         <v>42</v>
       </c>
       <c r="I52" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J52" s="26" t="s">
+      <c r="J52" s="21" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3216,6 +3244,7 @@
     <mergeCell ref="G34:G41"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3362,7 +3391,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3487,7 +3515,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3645,7 +3672,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>